<commit_message>
fix the error in saving data, the first web is scrapping successful
</commit_message>
<xml_diff>
--- a/recipes_df.xlsx
+++ b/recipes_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,30 +441,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ingredients</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>steps</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>diners</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>duration</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>difficulty</t>
         </is>
@@ -481,30 +486,35 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-champinones-rellenos-vegetarianos-75703.html</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Receta de Champiñones rellenos vegetarianos</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -521,30 +531,35 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-aceitunas-rebozadas-con-queso-75694.html</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Receta de Aceitunas rebozadas con queso</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>15m</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -561,30 +576,35 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepas-veganas-75645.html</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Receta de Arepas veganas</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Dificultad muy baja</t>
         </is>
@@ -601,30 +621,35 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-pan-de-ajo-keto-75668.html</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Receta de Pan de ajo keto</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>2 comensales</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -641,30 +666,35 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-torrejas-de-coliflor-75657.html</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Receta de Torrejas de coliflor</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -681,30 +711,35 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamales-de-pina-con-coco-75647.html</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Receta de Tamales de piña con coco</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>10 comensales</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -721,30 +756,35 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-empanadas-de-hamburguesa-75653.html</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Receta de Empanadas de hamburguesa</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>5 comensales</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -761,30 +801,35 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-torre-de-panqueques-salada-75659.html</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>Receta de Torre de panqueques salada</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -801,30 +846,35 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamales-de-calabaza-75649.html</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Receta de Tamales de calabaza</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>10 comensales</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -841,30 +891,35 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamales-de-nutella-75648.html</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Receta de Tamales de Nutella</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>10 comensales</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -881,30 +936,35 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamales-de-frijoles-75650.html</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Receta de Tamales de frijoles</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>['\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>15 comensales</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -921,22 +981,27 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/articulo-despierta-tu-sentido-iberico-75644.html</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Despierta tu Sentido Ibérico</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronomía para convertirse en todo un emblema cultural de la Dieta Mediterránea; un producto que despierta el interés por nuestro modo de vida y costumbres, así como por conocer una cultura gastronómica digna de ser declarada de interés cultural.Un minucioso, tradicional, natural y largo proceso de elaboración que culmina con el disfrute sensorial de un producto único. Para apreciar los matices dulces, salados y curados del Jamón Ibérico y gozar al máximo de esa explosión de sabor tan característica en nuestro paladar, debemos utilizar todos los sentidos: vista, tacto, olfato, gusto…Así surge el proyecto internacional “Jamones Ibéricos de España, Embajadores de Europa en el Mundo”. Una campaña emocional que impulsa ASICI, con el apoyo de la Unión Europea, con la que se persigue estimular al mundo entero para que despierte su Sentido Ibérico y se deleite con el sabor inconfundible de este producto gourmet único en el mundo.\n\n\n\n\n\n\n\n\n', '\nTienes un sentido que es la suma de todos. El Sentido Ibérico. Un sentido que nace en la cultura mediterránea, que nace de unir algo tan único como el Jamón Ibérico y algo tan extraordinario como una forma especial de entender y vivir la vida. Se trata de sentir, compartir y disfrutar. Porque el ‘Sentido Ibérico’ te lleva a la esencia de lo que somos… a percibir un aroma, un color o un sabor increíble, a disfrutar del Jamón Ibérico.\n', '\nEl Sentido Ibérico no se puede describir, solo se puede vivir porque hablamos de algo más que un alimento. Hablamos de cultura europea, de patrimonio gastronómico, de mundo rural, del paisaje que lo proporciona, de sostenibilidad… En definitiva, hablamos de un producto singular y especial.Un producto que necesita 4, 5, 6, 7… años antes de ser disfrutado. Porque si algo caracteriza el proceso de elaboración de un Jamón Ibérico es que es un proceso natural basado en largos tiempos de elaboración y curación. Un Jamón Ibérico necesita mucho tiempo para convertirse en una obra maestra. En un producto con un aroma intenso y persistente fruto de las fases finales de maduración, con un sugerente aspecto de color rojizo intenso dibujado por su veteado característico y con una textura firme que permite el corte en lonchas muy finas.Si estás dispuesto a esperar todo ese tiempo para disfrutar del aroma y el sabor inconfundible del Jamón Ibérico, es porque tienes el Sentido Ibérico. Está dentro de ti, no importa de dónde seas... lo tienes. Tan solo necesitas una loncha de Jamón ibérico para despertarlo.Despierta tu Sentido Ibérico. Jamones Ibéricos de España, embajadores de Europa en el mundo.\n\n\n\n\n\n\n\n\n', '\n*El contenido de la presente publicidad representa únicamente la opinión de su autor y es responsabilidad exclusiva del mismo. La Comisión Europea no asume ninguna responsabilidad por el uso que pudiera hacerse de la información que contiene.\n', '\nSi te ha gustado el artículo Despierta tu Sentido Ibérico, te sugerimos que entres en nuestra categoría de Otros aperitivos.\n']</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -949,30 +1014,35 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-empanadico-de-calabaza-75638.html</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>Receta de Empanadico de calabaza</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de empanadico de calabaza, primero añade en un bol todos los ingredientes de la masa, excepto el agua. Empieza a amasar y añade el agua poco a poco hasta que se forme una masa que se despegue del molde.\n\n\n\n\n\n', '\n2\nForma una bola, tapa y deja reposar aproximadamente 15-20 minutos.\n\n\n\n\n\n', '\n3\nLimpia el centro de la calabaza, para ello retira las pipas y la piel de fuera, seguido, corta en rodajas muy finas como si fuera para una tortilla de patatas.\n\n\n\n\n\n', '\n4\nEstira la masa con un rodillo proporcionando forma redonda o alargada. Señalamos que también se puede partir la masa en dos y hacer la empanada. Y, si te cuesta estirarla, puedes poner la masa en medio de dos hojas de papel vegetal y pasar el rodillo para que sea más fácil estirarla.\n\n\n\n\n\n', '\n5\nColoca una hoja de papel para horno encima la masa y a un lado añade la calabaza, las pasas, los piñones y espolvorea con azúcar y canela. Echa aceite de oliva por encima y añade otra capa de calabaza, pasas, piñones, azúcar y canela.\n\n\n\n\n\n', '\n6\nCierra la masa y sella los bordes con un tenedor como si fuera una empanadilla para que no se salga el relleno. Haz un agujero en el centro para que salga el aire al cocinarse. Luego, con los trozos de masa sobrantes añade unas tiras por encima del empanadico.\n\n\n\n\n\n', '\n7\nCon una brocha de cocina pinta la empanada con aceite de oliva y espolvorea con azúcar y canela.\n\n\n\n\n\n', '\n8\nPon a calentar el horno a 180 ºC con calor arriba y abajo. Cuando esté caliente, coloca la bandeja en el centro con la empanada y deja que se cocine aproximadamente 30 minutos o hasta que la masa esté dorada. Retira y deja enfriar. ¡Ya puedes disfrutar de esta receta de empanadico de calabaza! Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadico de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nValor nutricional de la calabaza\nLa calabaza tiene múltiples beneficios para la salud, estos son algunos de ellos:Refuerza las defensas.Beneficia la salud ocular.Cuida el sistema cardiovascular. Si te ha gustado esta receta de empanadico de calabaza y quieres conocer otras recetas similares, no te pierdas las siguientes elaboraciones:Empanadas de manzana y canelaEmpanada de champiñonesEmpanadas de calabaza y quesoEmpanadas de jurel\n', '\nSube la foto de tu Receta de Empanadico de calabaza\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Dificultad media</t>
         </is>
@@ -989,30 +1059,35 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-hallacas-navidenas-75631.html</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Receta de Hallacas navideñas</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>['\n1\nPara comenzar con la receta de hallacas navideñas fácil, primero es necesario tener todas las verduras picadas. La cebolla blanca en cuadrados pequeños, el poro en media luna, el cebollín, también conocido como cebolla china, corta en cuadrados pequeños, el ajo cortado finamente y el pimiento en tiras.\n\n\n\n\n\n', '\n2\nCocina la pechuga de pollo. Señalamos que se recomienda agregar un pedazo de poro o de apio en la cocción del pollo. Cuando esté listo, deshilacha y almacena, es importante no desechar el fondo de ave.\n\n\n\n\n\n', '\n3\nEn una olla mediana, agrega un chorro de aceite de achiote y añade la cebolla blanca en cuadrados. Cocina hasta que se encuentre transparente.\n\n\n\n\n\n', '\n4\nAñade el ajo cortado finamente y el poro.\n\n\n\n\n\n', '\n5\nSeguido, añade el cebollín y el pimiento. Mezcla con la ayuda de una cucharada y cocina aproximadamente 5 minutos a fuego bajo.\n\n\n\n\n\n', '\n6\nAñade la carne de res y la carne de cerdo. Mueve e incorpora la sal, la pimienta y el vino tinto. Deja que el alcohol del vino se evapore.\n\n\n\n\n\n', '\n7\nCuando ya no sientas olor a alcohol, añade media taza de caldo de pollo y deja cocinar aproximadamente 25 minutos.\n\n\n\n\n\n', '\n8\nDespués del tiempo indicado, agrega la pechuga de pollo previamente deshilachada.\n\n\n\n\n\n', '\n9\nEn un recipiente pequeño, agrega 1 cucharada de harina de maíz con un chorro de caldo de ave y diluye.\n\n\n\n\n\n', '\n10\nAñade el maíz disuelto en el guiso y mueve. Deja cocinar aproximadamente 4 minutos.\n\n\n\n\n\n', '\n11\nEn un bol mediano, añade la harina de maíz para la masa y una pizca de sal.\n\n\n\n\n\n', '\n12\nIncorpora 2 cucharadas de aceite de achiote y mueve con la ayuda de las manos.\n\n\n\n\n\n', '\n13\nPoco a poco añade el fondo de ave y forma una masa.\n\n\n\n\n\n', '\n14\nEstira las hojas de plátano, agrega una bola de masa y estirarla.\n\n\n\n\n\n', '\n15\nColoca el guiso, las aceitunas, el pimiento, las pasas y una lonja de tocino.\n\n\n\n\n\n', '\n16\nEnvuelve con otra hoja de plátano y amarrara con la ayuda de un pabilo. Lleva una olla a hervir con agua aproximadamente 30 minutos\n\n\n\n\n\n', '\n17\nDisfruta calientes las hallacas navideñas y cuéntanos en los comentarios qué te ha parecido esta receta venezolana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Hallacas navideñas, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nValor nutricional de las hallacas navideñas\nPor cada porción de hallaca (300 gramos aproximadamente) se encuentran 589 kcal, 41.1g de grasas, 32.84g de carbohidratos, 23.6g de proteína, 6.36g de azúcar, 2.9g de fibra, 3.18g de sal, 112 mg de colesterol y 576 mg de potasio.Si te ha gustado esta receta venezolana y quieres conocer otras elaboraciones similares para cocinar en Navidad, sigue leyendo:Romeritos navideñosHallacas vegetarianasTamales de rajasMixiotes navideños\n', '\nSube la foto de tu Receta de Hallacas navideñas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>20 comensales</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Dificultad media</t>
         </is>
@@ -1029,30 +1104,35 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-croquetas-de-calabaza-y-queso-75622.html</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Receta de Croquetas de calabaza y queso</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de croquetas de calabaza y queso, primero debes retirar la corteza y las pipas. Seguido, debes cortarla en trozos y cocinarla. Señalamos que la puedes cocinar en el horno asada, cocida o en el microondas. En esta ocasión, la hemos cocido en el microondas a máxima potencia, aproximadamente 7-8 minutos. Y, si con este tiempo no está suficientemente blanda, vuelve a ponerla en el microondas unos minutos más hasta que quede bien cocida. Tritúrala con la ayuda de un tenedor.\n\n\n\n\n\n', '\n2\nPica la cebolla muy pequeñita y coloca una sartén amplia en el fuego, añade un chorro de aceite de oliva y pocha la cebolla. Cuando ya esté bien pochada, añade la calabaza echa puré, mezcla bien y deja que adquiera el sabor de la cebolla. Añade un poco de sal y pimienta.\n\n\n\n\n\n', '\n3\nAñade el queso rallado y mézclalo todo. Puedes añadir la cantidad que prefieras según te guste la masa.\n\n\n\n\n\n', '\n4\nEn cuanto al queso, podéis añadir el que más os guste, pero es cierto que los quesos que se funden son ideales. Mezcla hasta que queden bien integrados todos los alimentos.\n\n\n\n\n\n', '\n5\nColoca la masa en una fuente y deja que se enfríe. Añade en la nevera unos minutos, también puedes dejarlo de un día para otro. Señalamos que también puedes elaborar las croquetas de calabaza y queso con bechamel. En este artículo de RecetasGratis te mostramos una receta deliciosa de bechamel con cebolla para añadir a tus croquetas si lo ves conveniente.\n\n\n\n\n\n', '\n6\nRetira la masa de la nevera y forma las croquetas. Para ello, coloca en un bol el huevo batido y en otro el pan rallado. Debes ir pasando las croquetas primero por el huevo y luego, por el pan rallado. Señalamos que las croquetas también las puedes elaborar como si fueran bolitas de calabaza fritas, estarán igual de deliciosas, solo cambiará la forma.\n\n\n\n\n\n', '\n7\nColoca una sartén al fuego con abundante aceite y cuando esté caliente, coloca con cuidado las croquetas en tandas. Déjalas que se vayan dorando por todos los lados. Destacamos que las croquetas de calabaza y queso al horno también están deliciosas. ¡Escoge la opción que más te guste, a la sartén o al horno!\n\n\n\n\n\n', '\n8\nUna vez estén doradas, retíralas y colócalas en un plato con papel de cocina para que absorba el exceso de aceite. ¡Ya puedes disfrutar de esta receta de croquetas de calabaza y queso! Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Croquetas de calabaza y queso, te sugerimos que entres en nuestra categoría de Recetas de Croquetas.\n', '\nPropiedades y beneficios de la calabaza\nEl consumo de calabaza tiene múltiples beneficios para la salud, como por ejemplo:Cuida el sistema cardiovascular.Beneficia la salud ocular.Perfecta para el aparato digestivo.Refuerza las defensas.Y, si quieres conocer más recetas con calabaza, no te pierdas las siguientes elaboraciones:Hamburguesas de calabazaPizza de calabazaRaviolis de calabazaLasaña de calabazaCrema de calabaza y puerros light\n', '\nSube la foto de tu Receta de Croquetas de calabaza y queso\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1069,30 +1149,35 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tequenos-de-lomo-saltado-75616.html</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>Receta de Tequeños de lomo saltado</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n']</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar la receta de tequeños de lomo saltado, primero es importante cortar todas las verduras y la carne en trocitos pequeños, de igual manera debes hacerlo con la cebolla morada. En el caso del ají amarillo, retira las venas y las semillas utilizando un cuchillo, córtalo en cuadrados pequeños del mismo tamaño que la cebolla. El perejil debe estar cortado finamente y el tomate en cuadrados pequeños también, no olvides retirar las semillas.\n\n\n\n\n\n', '\n2\nEn un sartén mediana, agrega un chorro de aceite vegetal a fuego alto y cuando empiece a humear, incorpora la carne de res y mueve para lograr que se selle.\n\n\n\n\n\n', '\n3\nAgrega el chorrito de sillao claro, pimienta y ajo molido. Sigue moviendo el lomo con ayuda de una cuchara o con el sartén. Cuando toda la carne se encuentre dorada retirarla y colocarla en un recipiente.\n\n\n\n\n\n', '\n4\nEn la misma sartén, agrega un chorrito de sillao claro y añade la cebolla morada en cuadrados. Saltea aproximadamente 2 minutos.\n\n\n\n\n\n', '\n5\nAñade el ají amarillo y el tomate.\n\n\n\n\n\n', '\n6\nPasados 5 minutos, agrega la carne y apaga el fuego.\n\n\n\n\n\n', '\n7\nFinalmente, añade el perejil cortado finamente y mezcla los ingredientes. Prueba el sabor y agrega sal si lo necesita.\n\n\n\n\n\n', '\n8\nBate un huevo y agrega una pizca de sal. En una lámina de wantán, coloca un trozo de queso y encima una cucharada de lomo saltado. Seguido, pinta los bordes de la masa con huevo. ¿Qué te está pareciendo esta receta de tequeños con lomo saltado?\n\n\n\n\n\n', '\n9\nCierra con cuidado y sella los bordes con la ayuda de un tenedor. ¡Ya casi está la receta de tequeños rellenos de lomo saltado!\n\n\n\n\n\n', '\n10\nEn una olla mediana, calienta el aceite vegetal a fuego medio y añade los tequeños. Retíralos cuando se encuentren dorados y colócalos en una rejilla de metal.\n\n\n\n\n\n', '\n11\nDisfruta de estos tequeños de lomo salteado y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tequeños de lomo saltado, te sugerimos que entres en nuestra categoría de Recetas de Tequeños.\n', '\nCon qué acompañar los tequeños de lomo saltado\nLos tequeños son muy populares en Perú y, actualmente, existen muchas maneras de rellenarlos. Estos son algunas de las recetas más conocidas:Tequeños de batataTequeños de chocolateTequeños de yucaTequeños sin glutenY, además, te proporcionamos diferentes elaboraciones para acompañar los tequeños de lomo saltado:Ají de rocotoAjí de polleríaAjí de huacatayAjí de cocona\n', '\nSube la foto de tu Receta de Tequeños de lomo saltado\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>5 comensales</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1109,30 +1194,35 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepas-vegetarianas-75605.html</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>Receta de Arepas vegetarianas</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n']</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de las arepas vegetarianas, primero debes preparar la masa. Para ello, agrega dos tazas de harina de maíz, aceite y la sal a un recipiente. Añade también agua y remueve con una cuchara a la vez, tratando así de que no se formen grumos. La masa debe quedar con consistencia y con cierta elasticidad.\n\n\n\n\n\n', '\n2\nEn la foto puedes observar como debe quedar la masa. Debes dejarla reposar 10 minutos para que la harina absorba el agua restante.\n\n\n\n\n\n', '\n3\nUna vez que la masa tenga la consistencia necesaria, procede a repartirla aproximadamente en diez partes iguales formando diez bollos.\n\n\n\n\n\n', '\n4\nEscoge un bollo y aplástalo, debes tener en cuenta que debe quedar con una forma circular y con un grosor de 1.5cm. Añádelo a la sartén a fuego medio-bajo y déjalo entre 5-8 minutos. No debes mover la arepa hasta que pase 5 minutos aproximadamente.\n\n\n\n\n\n', '\n5\nCuando veas que una de las partes está cocinada, debes darle la vuelta. Repite el proceso con la otra parte y retíralas. Déjalas reposar 10 minutos para poder abrirlas.\n\n\n\n\n\n', '\n6\nPara el relleno de las arepas vegetarianas, debes picar en brunoisse, es decir, en cubos pequeños, la cebolla, el morrón y el diente de ajo.\n\n\n\n\n\n', '\n7\nCalienta el aceite en la sartén a fuego alto y agrega el ajo, enseguida que dore, también añade el morrón y la cebolla.\n\n\n\n\n\n', '\n8\nPasados los 5 minutos aproximadamente, agrega el zuchini y la cebolla. Esta última debe estar bastante dorada.\n\n\n\n\n\n', '\n9\nDespués de condimentar y de que el zucchini se haya cocinado, baja el fuego y agrega los dos huevos. Empieza a remover con una cuchara. ¡Ya casi está la receta saludable de arepas vegetarianas!\n\n\n\n\n\n', '\n10\nCorta el tomate y pica la albahaca. Agrega estos dos ingredientes al resto del relleno.\n\n\n\n\n\n', '\n11\nAbre la arepa por el medio con un cuchillo y agrega el relleno en ella. ¡Ya puedes disfrutar de estas deliciosas arepas vegetarianas! Cuéntanos en los comentarios qué te ha parecido esta receta.Y, si eres vegano y quieres aprender a cocinar unas deliciosas arepas veganas, no te pierdas esta receta de arepas de brócoli.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas vegetarianas, te sugerimos que entres en nuestra categoría de Recetas de Arepas.\n', '\nOtros rellenos de las arepas vegetarianas\nAdemás de este relleno que te hemos propuesto, puedes rellenar las arepas vegetarianas con otros ingredientes, como por ejemplo: champiñones, espinacas, tofu, tomate deshidratado, quesos, entre otros. Esta receta es ideal para acompañar con distintas salsas, frijoles, verduras, quesos, entre otras elaboraciones. Y, si quieres conocer con qué salsa acompañar las arepas vegetarianas, sigue leyendo:Guasacaca venezolanaSalsa tampicoSalsa de cabralesSalsa machaSalsa sriracha\n', '\nSube la foto de tu Receta de Arepas vegetarianas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>2 comensales</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1149,30 +1239,35 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamales-de-rajas-75612.html</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>Receta de Tamales de rajas</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n']</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>['\n1\n¿Te preguntas cómo hacer tamales mexicanos? Esta receta es ideal para ti. Para empezar con la receta de tamales de rajas, primero prepara la masa. En un recipiente coloca la harina, la pizca de sal, el polvo para hornear y el fondo de verduras o agua, y la manteca vegetal, debes mezclar para integrar todo y reservar. Además, debes agregar poco a poco el fondo de verduras para que no quede tan aguada la masa.\n\n\n\n\n\n', '\n2\nLava las hojas de los tamales y déjalas suavizar en agua tibia aproximadamente unos 15 minutos.\n\n\n\n\n\n', '\n3\nPrepara el relleno de rajas y asa los chiles poblanos. Cuando estén completamente asados, límpialos bien, retira el tallo, las venas y las semillas, luego corta en julianas.\n\n\n\n\n\n', '\n4\nLicua los ingredientes: los jitomates, el trozo de cebolla, el diente de ajo y la ramita de cilantro con un poco de agua.\n\n\n\n\n\n', '\n5\nEn una olla con una cucharada de aceite sofríe las rajas de chile poblano. Opcionalmente, también puedes agregar una rajas de chile serrano para añadir picor.\n\n\n\n\n\n', '\n6\nCuando estén ligeramente doradas vierte la salsa de tomate, señalamos que debes pasarla por un colador. Sazona con sal y pimienta al gusto y deja que se reduzca el líquido. Reserva.\n\n\n\n\n\n', '\n7\nAhora es momento de armar los tamales. Escoge una hoja, coloca una cucharada de masa y agrega un poco de rajas y de queso. ¡Ya casi está la receta de tamales con queso!\n\n\n\n\n\n', '\n8\nCierra el tamal y repite el proceso hasta terminar con la masa. Dependiendo del tamaño te saldrán más o menos tamales, aproximadamente 20-25. Luego, lleva a cocinar al vapor aproximadamente 40 minutos.\n\n\n\n\n\n', '\n9\nCuando pase el tiempo establecido, ya podrás disfrutar de estos ricos tamales de rajas. ¡Cuéntanos en los comentarios qué te ha parecido esta receta de tamales de rajas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de rajas, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de rajas y otros ingredientes\nPreparar tamales siempre es muy sencillo, los pasos a seguir son prácticos y, sobre todo, los ingredientes son variados. En este caso por ejemplo puedes agregar también algunos granos de maíz o sustituir el queso por alguno de tu preferencia. Así que anímate a preparar esta receta de tamales de rajas, consiente a los que más quieres con un platillo mexicano y no olvides prepararlos para las próximas posadas navideñas. Acompáñalos con un rico café de olla o atole.Y, si además, quieres conocer otras recetas de tamales, no te pierdas las siguientes elaboraciones:Tamales de chipilín con polloTamales en salsa verdeTamales de zarzamora con queso cremaTamales coladosTamales de acelgaTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de rajas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>12 comensales</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1189,30 +1284,35 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-torrejas-de-choclo-75603.html</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>Receta de Torrejas de choclo</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n']</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con esta receta de torrejas de choclo es necesario tener todos los ingredientes listos. En el caso del maíz, con la ayuda de un cuchillo sepáralo de la coronta. Señalamos que en esta receta se ha utilizado maíz amarillo, pero se puede usar el blanco sin ningún problema. También debes rallar el queso utilizando un rallador delgado. Corta la parte blanca de la cebolla china en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nLleva el maíz a la licuadora con la mantequilla y licua, pero no en su totalidad.\n\n\n\n\n\n', '\n3\nAgrega un huevo y licua hasta que los ingredientes se integren bien.\n\n\n\n\n\n', '\n4\nColoca la mezcla en un recipiente y añade la cebolla china picada.\n\n\n\n\n\n', '\n5\nAñade el queso rallado y mueve con la ayuda de una cuchara hasta que se forme una masa homogénea para elaborar las torticas de mazorca. Salpimienta al gusto.\n\n\n\n\n\n', '\n6\nEn una sartén antiadherente agrega un poco de mantequilla a fuego medio y una cucharada de masa, cuando el borde de la torreja empiece a secarse, debes darle la vuelta con mucho cuidado. Puedes utilizar una espátula de cocina. ¡Ya casi están las torrejas de maíz!\n\n\n\n\n\n', '\n7\nSirve como acompañamiento de algún plato o con ají criollo. ¡Ya puedes disfrutar de estas torrejas de choclo! Cuéntanos en los comentarios qué te ha parecido esta receta fácil.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de choclo, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nCon qué acompañar las torrejas de choclo\nPor cada 100 gramos de maíz se encuentran: 86 kcal, 19 g de carbohidratos, 1.2g de grasas, 3.2g de proteínas y 270 mg de potasio. Este alimento es una gran fuente de antioxidantes que ayudan a combatir el envejecimiento celular. Asimismo, la vitamina B1 que contiene disminuye la homocisteína, también contiene ácido fólico.Si te preguntas con qué acompañar las tortillas de choclo, no te pierdas estas salsas fáciles:Ají de rocotoAjí de polleríaAjí de huacatayAjí de coconaSi eres un gran amante del choclo y quieres conocer otras recetas con este ingrediente, sigue leyendo:Choclo con quesoTarta de chocloTorta de chocloPastel de maíz fácil caseroTortilla de choclosTortitas de choclos dulcesPastel de choclo con queso\n', '\nSube la foto de tu Receta de Torrejas de choclo\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1229,30 +1329,35 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-yuquitas-fritas-75582.html</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Receta de Yuquitas fritas</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n']</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de yuquitas peruanas, primero es necesario pesar todos los ingredientes con la ayuda de una balanza. Luego, debes mezclar la sal y el polvo de hornear con la harina. Después, debes añadir los granos de anís en agua hirviendo.\n\n\n\n\n\n', '\n2\nMezcla la levadura seca con la infusión de anís y el azúcar moreno. Señalamos que es importante que la infusión se encuentre tibia. Deja fermentar aproximadamente unos 5 minutos.\n\n\n\n\n\n', '\n3\nEn el bol de la harina incorpora el aceite vegetal y la levadura fermentada.\n\n\n\n\n\n', '\n4\nAmasa aproximadamente unos 10 minutos y coloca la masa en un recipiente. Deja reposar aproximadamente 1 hora.\n\n\n\n\n\n', '\n5\nCuando la masa haya reposado, estírala en forma de cilindro.\n\n\n\n\n\n', '\n6\nCorta tiras pequeñas de aproximadamente 9 cm, estíralas y realizar un corte en el centro con la ayuda de un cuchillo.\n\n\n\n\n\n', '\n7\nLleva las yuquitas a una olla con aceite caliente y cocina 2 minutos aproximadamente por cada lado. Retira y coloca en un colador metálico. ¡Ya casi está la receta de yuquitas fritas!\n\n\n\n\n\n', '\n8\n¡Ya puedes servir las yuquitas fritas peruanas de carretillas! Disfruta de este snack y cuéntanos en los comentarios qué te ha parecido.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Yuquitas fritas, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nCon qué acompañar las yuquitas fritas\nEl anís se emplea como potenciador de sabores en diversas preparaciones, tanto saladas como dulces. También se utiliza en forma de infusión para calmar dolores en el sistema digestivo, contiene zinc, fósforo, calcio y potasio. Señalamos que 100 gramos de semilla de anís tiene: 337 kcal, 17.6g de proteína y 50 gramos de hidrato de carbono.Si te preguntas con qué acompañar la yuca frita, tenemos la respuesta. Las yuquitas fritas se suelen acompañar con champú de piña, un delicioso postre típico en Lima, Lambayeque y Piura, también se puede acompañar con diferentes salsas peruanas, como por ejemplo:Ají de rocotoAjí de polleríaSalsa huancaína\n', '\nSube la foto de tu Receta de Yuquitas fritas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Dificultad muy baja</t>
         </is>
@@ -1269,22 +1374,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/articulo-ideas-de-aperitivos-para-halloween-75545.html</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>Ideas de aperitivos para Halloween</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['\nLas hamburguesas pueden convertirse en una divertida comida de Halloween, por eso mientras experimentábamos en la cocina, cobraron vida y se convirtieron en estos simpáticos monstruos. Seguro serán del gusto de tus hijos o sobrinos y así podrás brindarles durante ese día un almuerzo o cena de miedo, pero si esperas invitados, mejor prepara las hamburguesas en versión mini.¿Te gusta esta idea? Pues, corre a la cocina y ponla en práctica siguiendo el paso a paso de hamburguesas para niños. ¡Unos monstruos llenos de sabor! Ahora bien, si hay niños celiacos y no tienes tiempo para comprar o preparar pan sin gluten, puedes elaborarlas solo con la carne y adornarla, así como te indicamos en esta receta de hamburguesas para Halloween. ¡Calabazas de carne y queso!\n\n\n\n\n\n\n\n\n', '\nLas primeras manzanas acarameladas o confitadas se crearon en Norteamérica (EEUU) en 1908, pero no fue hasta mediado de los años 60 cuando se popularizaron como postres de Halloween. Nosotros tenemos dos alternativas para ti, una consiste en la receta clásica con caramelo y la otra en una preparación con chamoy, señalamos que su sabor dulce y ácido a la vez gustará a todos.Déjate llevar por el entusiasmo de esta festividad y prepara cualquiera de estas recetas, puedes empezar siguiendo los pasos de manzanas con chamoy o si prefieres la receta tradicional, sigue nuestras indicaciones de manzanas caramelizadas. ¡Un postre para grandes y chicos!\n\n\n\n\n\n\n\n\n', '\nQuien pensaría que entre tantas recetas saladas para Halloween, desempolvaríamos a unas momias de hojaldre y salchicha crujientes por fuera y jugosas por dentro. Si quieres que hipnoticen a tus comensales tras cada mordisco, solo sigue los pasos de la receta de momias de salchichas y hojaldre. ¡Fáciles y aterradoras!\n\n\n\n\n\n\n\n\n', '\nUna mesa de aperitivos para la fiesta de Halloween no queda completa si no introduces opciones dulces, especialmente si se trata de una fiesta infantil. Pensando en eso hemos decidimos aprovechar la versatilidad del merengue para crear unos huesitos muy vistosos y fáciles. Además estos aperitivos pueden servirte para decorar un bizcocho o unos cupcakes. ¡Quedan geniales!No se diga más, ponte el mandil y alista los ingredientes necesarios, pues en unos pocos pasos tendrás unos huesitos de merengue.\n\n\n\n\n\n\n\n\n', '\n¿Un perrito caliente como si fuera un dedo de zombi? Sí, estos aperitivos para la fiesta de Halloween son una propuesta muy creativa, y lucen tan reales que te darán escalofríos. Además, no necesitas de un gran presupuesto para prepararlos, pues tan solo contienen cuatro ingredientes accesibles: pan, salchichas y dos salsas.¿Quieres aprender a elaborarlos? Pues solo sigue los siguientes pasos fáciles de dedos de salchicha para Halloween. ¡Aterradoramente deliciosos! Ahora bien, si prefieres ver la receta en un vídeo junto con otras ideas ingeniosas, entonces échale un vistazo a la receta de Halloween para niños (3 recetas fáciles y rápidas).\n\n\n\n\n\n\n\n\n', '\nSi quieres postres de Halloween realmente creativos, solo necesitaras dar rienda suelta a tu imaginación y un poco de paciencia. Basándonos en lo que hemos comentado anteriormente, transformamos unos brownies normales en lápidas, tan solo dándole forma a las puntas de uno de sus extremos.Ahora bien, se nos ocurre que también puedes usar unos cortapastas o moldes de cartulina creados por ti (para recortar los brownies con cuchillo), y así obtener otras figuras adicionales, por ejemplo: esqueletos (usando un cortapastas de muñeco de jengibre), calaveras, murciélagos, pentagramas (a partir de un cortapastas de estrella), manos tenebrosas, y muchas otras. Una vez terminados, decoras con glasé blanco, quedarán geniales, pues ambos tonos contrastan. ¿Qué esperas para divertirte? Solo junta los ingredientes y utensilios necesarios mientras sigues los pasos de brownie decorado. ¡Pura dulzura tenebrosa!\n\n\n\n\n\n\n\n\n', '\nSi aún no tienes planeada una fiesta para tus peques, consiéntelos al menos con una cena de Halloween en casa. ¡Y qué mejor sorpresa que una pizza con una presentación muy especial!Prepara una pizza tamaño familiar o mejor varias pequeñas y decora con motivos terroríficos tales como fantasmas, momias, dedos o arañas. ¿Qué decoración añadirías tú? Pues deja tu imaginación volar mientras sigues los pasos de pizza de Halloween para niños o la versión mini siguiendo las instrucciones de pizzas de Halloween. ¡Puro sabor espectral!\n\n\n\n\n\n\n\n\n', '\nYa sabes que los cakes pops son geniales como aperitivos para fiestas de Halloween, especialmente si se trata de una fiesta infantil. Partiendo de esa idea, te proporcionamos una receta de unos murciélagos de miedo, vistosos y gustosos. Dales vida siguiendo el paso a paso de cake pops para Halloween de murciélagos.¿Otras sugerencias? Cubre los cakes pops con chocolate blanco o ponles fondant y dibújales los detalles con marcadores comestibles o trocitos de fondant, así obtendrás diseños geniales. Por ejemplo, nosotros te proponemos una idea muy divertida, un fantasmita hecho con un círculo de fondant blanco. Ese círculo debes acomodarlo sobre el cake pops y apretarlo un poco para crear los pliegues de la sábana, después puedes ponerle los ojitos y listo. ¡Te encantará!\n\n\n\n\n\n\n\n\n', '\nComo ves, los snacks salados caseros son muy divertidos, y además, puedes hacerlos más ligeros si usas solo productos bajos en calorías. Ahora bien, si empleas varios tipos de pan negro (con pasas, zanahoria, cereales u otros) y le das formas diversas a cada uno (calaveras, gato, búho, arañas, lápidas, etc.), obtendrás una gran variedad de botanas económicas.Solo te queda elegir variedad de dips y seguir el paso a paso de esta receta de escobas de bruja con queso para Halloween. ¡Unos aperitivos espeluznantes!\n\n\n\n\n\n\n\n\n', '\nTenemos un reto muy divertido para tu fiesta de Halloween inspirado en la famosa serie titulada El juego del calamar, pero totalmente inofensivo. El jugador que logre sacar la figura central del Dalgona Candy sin romperlo, ganará un premio al finalizar la fiesta (un videojuego, una bolsa de chucherías, etc.). ¿Y los perdedores? Ellos solo se deleitarán con este sabroso dulce coreano. ¿Nada mal verdad? Pues no esperes más y disfruta de uno de nuestros mejores postres de Halloween siguiendo cada paso de Dalgona Candy.\n\n\n\n\n\n\n\n\n', '\nEstos postres de Halloween consisten en unas tumbas hechas de mousse de chocolate y galletas Oreo. Y además, te proporcionamos dos versiones, una con lápidas de galleta y otra con gusanos de gelatina arrastrándose por doquier.¿Con cuál te quedas? Nosotros pensamos que puedes elaborar las dos siguiendo el paso a paso de mousse de chocolate para Halloween y siguiendo también la receta de gusanos de gelatina y chocolate.\n\n\n\n\n\n\n\n\n', '\nUnos monstruos muy coloridos y divertidos dejaron estos snacks salados saludables y ahora nosotros los compartimos contigo en el siguiente paso a paso fácil de huevos cocidos para niños-dinosaurios (sirven huevos de gallina o de codorniz). ¡Completarán tu terrorífica mesa!Además, también aparecieron por arte de magia unos huevos con sorpresas espeluznantes, las cuales puedes descubrir preparando los huevos rellenos para Halloween.\n\n\n\n\n\n\n\n\n', '\nEstos fantasmas no asustan, pero deleitan el paladar, por eso no podían pasar inadvertidos como parte de los mejores aperitivos para fiesta de Halloween. Además, prepararlos es muy sencillo si sigues el paso a paso de fantasmas de merengue para Halloween. ¡Fáciles y deliciosos!\n\n\n\n\n\n\n\n\n', '\nLas palomitas de maíz son económicas y versátiles, es por eso que funcionan muy bien como aperitivos para fiesta de Halloween. A partir de esa idea, nos inspiramos y obtuvimos como resultado unos cerebros aterradoramente dulces hechos de malvaviscos. La receta es muy fácil y queda lista en dos por tres si sigues el paso a paso de palomitas de maíz para Halloween.\n\n\n\n\n\n\n\n\n', '\nSi todavía te falta inspiración, aquí te dejamos más recetas de Halloween llenas de creatividad. Hay infinidad de ideas, incluso algunas preparaciones sin decoración, pero con los sabores predilectos de esta temporada. No te pierdas estas recetas que te proporcionamos a continuación:Palomitas de Oreo y chocolate blancoPalomitas dulces de sarténPalomitas de coloresBombones decorados para HalloweenCake pops para Halloween de arañasDulces de leche para HalloweenTrufas de chocolate para niños-postres para HalloweenBrochetas de chuches para niñosOjos de gelatinaHuevos rellenos para niñosPostre de oreo-postre con gusanos para niñosPonche sangriento para HalloweenRollos de calabaza y canelaBuñuelos de manzana\n', '\nSi te ha gustado el artículo Ideas de aperitivos para Halloween, te sugerimos que entres en nuestra categoría de Otros aperitivos.\n']</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1297,30 +1407,35 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-mil-hojas-de-foie-con-manzana-y-cebolla-caramelizada-75528.html</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>Receta de Mil hojas de foie con manzana y cebolla caramelizada</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n']</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>['\n1\nLo primero que debes hacer para preparar el mil hojas de foie es cocinar la cebolla caramelizada. Pues bien, pela la cebolla, córtala en tiras finas y colócala en una sartén con unas cucharadas de aceite. Añade un poco de sal y tapa la sartén para que se cocine a fuego muy suave durante 20 minutos.\n\n\n\n\n\n', '\n2\nPasados los 20 minutos, la cebolla debe estar transparente y con color, sube el fuego un poco más. Añade 2 cucharadas de agua y el azúcar, la cantidad es al gusto, según el dulzor. Una vez has añadido el azúcar, debes remover sin parar para que la cebolla se vaya caramelizando.\n\n\n\n\n\n', '\n3\nDeja que se vaya cocinando hasta que quede bien caramelizada, añade agua si ves que le hace falta.\n\n\n\n\n\n', '\n4\nLava la manzana y con un cuchillo o con una mandolina corta láminas de manzana. Colócala en un plato e introduce en el microondas a máxima potencia unos segundos para que quede blanda.\n\n\n\n\n\n', '\n5\nEl foie debes reservarlo en la nevera hasta la hora de utilizarlo para que no se ablande mucho y se pueda cortar con facilidad. Debes cortarlo en rodajas de medio centímetro. ¡Ya casi esta el mil hojas de foie con manzana y cebolla caramelizada!\n\n\n\n\n\n', '\n6\nEscoge moldes redondos o cuadrados y coloca primero una capa fina de manzana, debe cubrir todo el fondo. Seguido añade una capa de foie, otra de manzana y otra de foie.\n\n\n\n\n\n', '\n7\nTermina con una capa de manzana y encima añade un poco de cebolla caramelizada. Añade también un poco de vinagre balsámico alrededor y acompaña con unas tostaditas de pan. ¡A comer la receta de mil hojas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Mil hojas de foie con manzana y cebolla caramelizada, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nMil hojas de foie con manzana y cebolla caramelizada y otras recetas\nEsta receta de mil hojas de foie con manzana y cebolla caramelizada se puede tener preparada con antelación y reservar en la nevera, ya que enseguida se ablanda el foie. Señalamos también que en vez de hacer el mil hojas individual se puede hacer con un molde más grande y queda muy vistoso. Además, queremos destacar que el hojaldre de foie y manzana, el milhojas de foie y queso de cabra y la lasaña de foie y manzana, son platos muy populares y deliciosos que seguro que también te encantarán.Si te ha gustado el timbal de foie con manzana y quieres conocer otros platillos deliciosos, no te pierdas las siguientes recetas:Timbal de bacalaoTimbal de calabacín y tomateTimbal de verduras a la planchaSolomillo con foie y manzanaManzanas caramelizadasTimbal de manzana con Thermomix\n', '\nSube la foto de tu Receta de Mil hojas de foie con manzana y cebolla caramelizada\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>2 comensales</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1337,30 +1452,35 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-croquetas-de-papa-75532.html</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>Receta de Croquetas de papa</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n']</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>['\n1\nPara hacer la receta de croquetas de papa, primero debes cocinar las papas con una pizca de sal y suficiente agua hasta que estén suaves. El tiempo dependerá del método de cocción que elijas, puede ser en una olla a presión o en una olla normal, pero ten en cuenta que deben estar suficientemente suaves.\n\n\n\n\n\n', '\n2\nCuando las papas estén listas, retira la piel y empieza a machacar, luego agrega 1 cucharada de mantequilla, 1 cucharada de queso parmesano o queso panela rallado, 1 pizca de ajo en polvo, 1 pizca de pimienta y una pizca de perejil seco, mezcla muy bien hasta integrar todos los ingredientes.\n\n\n\n\n\n', '\n3\nPara armar las croquetas de papa rellenas prepara todos los ingredientes en un recipiente y mezcla los huevos con la leche. Además, para el relleno debes cortar cubos de queso. Finalmente, prepara un plato con harina y otro con pan molido.\n\n\n\n\n\n', '\n4\nForma bolitas con la papa, toma una porción de queso, rellena, cierra y dale forma.\n\n\n\n\n\n', '\n5\nProcede a pasar la bolita de papa por la harina, enseguida por el huevo con leche y por último debes rebozar la croqueta por el panko o pan molido. Puedes repetir una o dos veces más el proceso para que quede una costra de pan más gruesa. ¡Ya casi están listas las croquetas de papa fáciles!\n\n\n\n\n\n', '\n6\nEn una olla con suficiente aceite caliente, fríe las croquetas aproximadamente unos 3 minutos. Señalamos que puede permanecer en la olla o sartén menos tiempo, solo debes cuidar que no se quemen. Cuando estén fritas retira el aceite y deja reposar sobre una rejilla o plato con papel absorbente.\n\n\n\n\n\n', '\n7\nLista la receta de croquetas de papa, así de sencillo es preparar este plato. Acompaña con ensalada o disfruta con aderezo o con salsa de tu preferencia. ¡A comer!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Croquetas de papa, te sugerimos que entres en nuestra categoría de Recetas de Croquetas.\n', '\nLos mejores tips para las croquetas de papa\nPreparar esta receta es muy fácil y el resultado te quedará increíblemente crujiente, de verdad que no te arrepentirás del sabor de estas croquetas de papa. Y además, como lo mencionamos anteriormente, te proporcionamos los mejores tips para que el resultado sea exquisito:Utiliza panko para rebozar las croquetas, este aportará una textura mucho más crujiente que el pan molido tradicional. Si no encuentras panko, también puedes buscar pan molido crujiente, puedes encontrarlo en los supermercados.Para que esté más suave y cremoso el puré de papa añade mantequilla.Agrega las especias que más te gusten, puedes probar añadiendo diferentes como por ejemplo: paprika, pimienta, tomillo u orégano.Para el relleno puedes utilizar queso panela en cubos, queso manchego o chihuahua, o bien puedes optar por un relleno de carne o pollo molido.Si te ha gustado esta receta y quieres aprender a elaborar otras preparaciones, te proporcionamos alternativas:Croquetas de atún con papaCroquetas de patata y quesoCroquetas de papa al hornoCroquetas de jamón serranoCroquetas de patata y jamón\n', '\nSube la foto de tu Receta de Croquetas de papa\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1377,30 +1497,35 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-croquetas-de-papa-al-horno-75526.html</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>Receta de Croquetas de papa al horno</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n']</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>['\n1\nEl primer paso que debes hacer para elaborar esta receta de croquetas de papa al horno es cocinar la papa. Para ello, cepilla la papa y pínchala con su cáscara. Cocínala en el microondas aproximadamente unos 4-5 minutos de cada lado.\n\n\n\n\n\n', '\n2\nCon cuidado de no quemarte, quítale la piel a la papa para tus deliciosas croquetas.\n\n\n\n\n\n', '\n3\nPísala y condiméntala al gusto. Señalamos que la nuez moscada y la pimienta combinan muy bien con la papa. Sin embargo, también puedes agregar mostaza, ajo en polvo, romero, cebolla de verdeo picada, entre otras opciones.\n\n\n\n\n\n', '\n4\nUna vez que el puré esté frío, toma pequeñas cantidades con la ayuda de una cuchara, rellénala con queso y ciérrala. Procede a rebozarlas pasándolas primero por huevo y luego por el pan rallado mezclado con la polenta. Repite el rebozado para que quede bien sellado y no se pierda el queso. Señalamos que puedes darle a tus croquetas la forma que desees: redondas, cilíndricas, cuadradas, a tu gusto. Enciende el horno fuerte a 200 ºC.\n\n\n\n\n\n', '\n5\nDispón las croquetas en una asadera con rocío vegetal o 1 cucharadita de aceite desparramada o con la servilleta. Cocínalas en el horno fuerte precalentado aproximadamente 12 minutos. ¡Ya casi están listas las croquetas de puré de patata al horno!\n\n\n\n\n\n', '\n6\nUna vez pasado ese tiempo, gira tus croquetas y cocínalas 3-5 minutos más para que se doren de forma pareja.\n\n\n\n\n\n', '\n7\n¡Sírvelas y disfruta de estas deliciosas y crocantes croquetas de papa fáciles!¿Qué te ha parecido esta receta de croquetas de patatas rellenas de queso? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Croquetas de papa al horno, te sugerimos que entres en nuestra categoría de Recetas de Croquetas.\n', '\nCroquetas de papa al horno light y otras versiones\nPuedes reemplazar el queso fresco para rellenar la papa por queso azul, morcilla, jamón, atún o pollo. Además, en nuestra web encontrarás miles de opciones de croquetas para disfrutar, es por eso que si te ha gustado esta receta de croquetas, te proporcionamos alternativas deliciosas:Croquetas de calabazaCroquetas de atún con papaCroquetas de morcillaCroquetas de papa y queso cremaCroquetas de jamón serranoCroquetas de patata y queso\n', '\nSube la foto de tu Receta de Croquetas de papa al horno\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1417,30 +1542,35 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tamalitos-verdes-75473.html</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>Receta de Tamalitos verdes</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n']</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar a preparar los tamalitoz verdes, corta en pequeñas partes el cerdo y sazona con sal y pimienta al gusto. Calienta en una olla pequeña el aceite y fríe todo el chancho, logrando que quede como chicharrón. Este aceite donde freíste el chicharrón, resérvalo.\n\n\n\n\n\n', '\n2\nPor otro lado, alista el choclo desgranado. Recuerda que mientras más fresco, el resultado será muchísimo mejor.\n\n\n\n\n\n', '\n3\nTambién separa las hojas de culantro. Al igual que el choclo, trata de conseguir el culantro más fresco que haya, esto hará que los tamalitos verdes consigan el color y aroma que lo caracteriza.\n\n\n\n\n\n', '\n4\nLimpia bien y enjuaga los ajíes amarillos para evitar que el resultado sea muy picante.\n\n\n\n\n\n', '\n5\nEs hora de empezar a procesar todos los ingredientes. Con ayuda de un molino o un procesador de alimentos, ve colocando poco a poco el choclo, el culantro, el ají amarillo y el chancho hasta obtener una mezcla pastosa.\n\n\n\n\n\n', '\n6\nAl terminar de procesar todos los ingredientes, añade sal y pimienta al gusto y mueve ligeramente la mezcla.\n\n\n\n\n\n', '\n7\nEcha a la mezcla el aceite de la fritura del cerdo que reservaste en el paso 1. Mezcla suavemente y prueba finalmente el nivel de sal.\n\n\n\n\n\n', '\n8\nEn una olla grande, ve calentando agua hasta la mitad. Aquí es donde pondrás luego a cocinar los tamales. Ahora es momento de armar los tamalitos verdes. Abre cuidadosamente las pancas, une dos de ellas por el lado más ancho y empieza a poner sobre ellas una buena porción de la mezcla, tal y como lo puedes ver en la imagen.\n\n\n\n\n\n', '\n9\nUna vez rellenos, envuelve con cuidado cada lado del tamal y luego junta las puntas de ambas pancas para lograr la forma siguiente.\n\n\n\n\n\n', '\n10\nCon ayuda de tiras de pabilo o alguna cuerda delgada con la que puedas amarrar, asegura cada tamal, de tal forma que al momento de la cocción no se desarmen.\n\n\n\n\n\n', '\n11\nRellenos, envueltos y amarrados todos los tamales, llévalos a cocinar dentro de agua hirviendo, la que previamente dejaste calentando. Coloca cuidadosamente uno sobre otro dentro de la olla.\n\n\n\n\n\n', '\n12\nSi te han sobrado pancas, puedes colocarlas arriba de todos los tamales, haciendo las veces de techo para que la cocción sea más uniforme dentro de la olla. Deja cocinando los tamalitos verdes por alrededor de una hora.\n\n\n\n\n\n', '\n13\nPasada la hora de cocción, ya estarán listos nuestros tamalitos verdes peruanos. Deberán quedar de una textura compacta, pero suave al probarla. Retira todos los tamales de la olla y deja enfriar por unos minutos antes de abrir y servir. Puedes acompañarlos con una zarza criolla. También es muy recomendado servirlo como acompañamiento de muchos platos criollos peruanos, como este: "Sopa seca chinchana".\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamalitos verdes, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas peruanas.\n', '\nFotos de Tamalitos verdes\n\n\n\n\n', '\nSube la foto de tu Receta de Tamalitos verdes\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>10 comensales</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>Dificultad media</t>
         </is>
@@ -1457,30 +1587,35 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepa-sifrina-75485.html</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>Receta de Arepa sifrina</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n']</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>['\n1\nComienza la preparación de estas deliciosas arepas sifrinas cocinando el pollo. Para ello, corta la cebolla y las zanahorias en pluma y bastones, respectivamente. Puedes hacer cortes grandes, ya que la cocción será larga y se cocinarán por completo. Haz un colchón con las verduras y el vino sobre una asadera para horno. Sobre ellas, coloca las presas de pollo y cúbrelas con el orégano y el limón cortado en rodajas.Cocina esta preparación al horno a 200 ºC por aproximadamente 1 hora o hasta que toda la carne esté completamente cocida.\n\n\n\n\n\n', '\n2\nCuando tengas el pollo bien cocido, procede a desmecharlo con ayuda de un cuchillo y tenedor, descartando los cartílagos y los restos de piel para no encontrarlos en tu relleno. Luego, déjalo enfriar.\n\n\n\n\n\n', '\n3\nMezcla el pollo desmechado con la mayonesa y el aguacate cortado en cubos. Si quieres, puedes condimentarlo con sal y pimienta.\n\n\n\n\n\n', '\n4\nCalienta tus arepas y córtalas por el medio, sin llegar hasta el final. Debería quedar como un libro. Rellénalas con esta preparación de pollo desmechado, mayonesa y aguacate. Distribuye en cada una el queso amarillo rallado y disfruta de estas deliciosas arepas sifrinas. Si pruebas esta receta, no dudes en compartir con nosotros la foto de tu plato en los comentarios, ¡Nos encantaría verla!¿No sabes cómo hacer la masa de arepas? No te pierdas nuestra Receta de arepas de maíz.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepa sifrina, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nTruco para hacer arepa sifrina más rápido\nSi deseas reducir los tiempos de esta preparación, podrías hervir el pollo con apio, zanahoria y ajo, en lugar de cocinarlo al horno.¡Encuentra en la web muchas ideas más de rellenos para arepas! Consulta nuestro artículo sobre los diferentes Tipos de arepas y prepara distintas versiones.\n', '\nFotos de Arepa sifrina\n\n\n\n', '\nSube la foto de tu Receta de Arepa sifrina\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1497,30 +1632,35 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepa-pelua-75482.html</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>Receta de Arepa pelúa</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n']</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>['\n1\nEmpieza la preparación de la arepa pelúa con la limpieza, pelado y cortado de los vegetales. Puedes cortarlos groseramente, ya que la cocción será larga y, de lo contrario, se desharán. Con ellos, haz un colchón cubriendo la base de una asadera para horno.\n\n\n\n\n\n', '\n2\nContinúa con la cocción del ingrediente estrella: la carne. Retírale la grasa visible y séllala en una sartén con aceite o rocío vegetal y el diente de ajo a fuego fuerte. Cuando esté dorada por todas sus partes, apóyala sobre el colchón de vegetales que preparaste en el paso anterior.\n\n\n\n\n\n', '\n3\nSin apagar el fuego, levanta el fondo de cocción de la carne con la copa de vino y los condimentos. Mientras, precalienta el horno a 180 ºC.\n\n\n\n\n\n', '\n4\nUna vez que no sientas olor a alcohol, vuelca la reducción del vino y los condimentos sobre la carne sellada y el colchón de vegetales. Sin duda, esta reducción aporta a la arepa pelúa muchísimo sabor.\n\n\n\n\n\n', '\n5\nTapa la asadera con la carne y los vegetales con papel de aluminio y cocínala en el horno medio precalentado a 180 ºC, por aproximadamente 1 hora y media. Cuando esté lista, los vegetales deberían deshacerse, la carne debería cortarse sin necesidad de cuchillo y los jugos deberían ser completamente marrones. Si logras este punto antes de la hora y media, puedes reducir el tiempo de cocción. Dependerá de tu horno y de lo ancho de la carne que estés utilizando.\n\n\n\n\n\n', '\n6\nProcede a desmechar la carne con ayuda de un tenedor para generar el efecto "pelúa". Pisa o corta los vegetales acompañando esta forma para que le aporten mayor jugosidad a la preparación.\n\n\n\n\n\n', '\n7\nCalienta tus arepas y córtalas por el medio, sin llegar hasta el borde. Deberían quedar como un libro. Rellénalas con la carne desmechada y el queso amarillo rallado. ¡A comer! Si pruebas esta receta de arepa pelúa, no dejes de compartir con nosotros la foto de tu plato terminado.Prepara tus propias arepas siguiendo la Receta de arepas de maíz. Además, descubre todos los tipos de arepas en este otro artículo.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepa pelúa, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nFotos de Arepa pelúa\n\n\n\n', '\nSube la foto de tu Receta de Arepa pelúa\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>3 comensales</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>2h 30m</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1537,30 +1677,35 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepa-perico-75483.html</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>Receta de Arepa perico</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n']</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>['\n1\nEmpieza la preparación del relleno de tu arepa perico picando los vegetales. Saltea la cebolla, el ají rojo y el diente de ajo en una sartén con el fuego fuerte y 1 cucharadita de aceite o rocío vegetal. Una vez que empiecen a dorarse, baja el fuego a medio y agrega 1 cucharadita de agua. Cuando se evapore, puedes agregar 1 cucharadita más y repetirlo tantas veces como quieras en función de lo cocida que te guste la verdura.\n\n\n\n\n\n', '\n2\nUna vez que hayas logrado el punto de cocción de tus vegetales deseado, agrega el tomate lavado y cortado en cubos y el huevo. Revuelve constantemente por 2 minutos para que el huevo se cocine y retira tu preparación del fuego.\n\n\n\n\n\n', '\n3\nProcede a calentar, cortar y rellenar tu arepa con este delicioso y fácil relleno húmedo. Al cortar la arepa, asegúrate de no llegar hasta el final, puesto que debe quedar como un libro. ¿Has visto qué fácil es hacer la arepa perico? Cuéntanos en los comentarios si lo has intentado y recuerda que también puedes adjuntar la foto del resultado. ¡Nos encantaría verlo!Prepara tus propias arepas caseras con esta sencilla Receta de arepas de maíz.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepa perico, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtras versiones de la arepa perico\nSi lo deseas, puedes agregar al salteado cebolla de verdeo y condimentos como comino, pimienta y sal. De hecho, al agregar verdeo, sumas más colores e imitas mejor al perico. Desde lo nutricional, cuanto más colores haya en el plato, más variedad de nutrientes también habrá.La combinación de hidratos presentes en la arepa, proteínas del huevo, grasas de la yema y fibra de los vegetales, le otorgan a este plato un valor de saciedad muy alto. Esto quiere decir que permanecerá más tiempo en tu estómago y hará que llegues con menos hambre a la comida siguiente, pudiendo moderar en ella la porción. Además, la combinación de fibra y proteínas con los hidratos de la arepa ayudan a que el aumento de la glucemia postprandial sea progresivo, disminuyendo la producción de grasas en el cuerpo.No te pierdas todas las ideas de rellenos para tus arepas que tenemos en nuestra web consultado el artículo sobre los Tipos de arepas. ¡A comer!\n', '\nFotos de Arepa perico\n\n\n\n', '\nSube la foto de tu Receta de Arepa perico\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>2 comensales</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>15m</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>Dificultad muy baja</t>
         </is>
@@ -1577,30 +1722,35 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepa-paisa-75481.html</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>Receta de Arepa paisa</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n']</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>['\n1\nComienza a preparar tus arepas paisa mezclando el agua con la harina. Debe quedar una mezcla húmeda, pero consistente. De ser necesario, corrige con más agua o harina para lograrla.\n\n\n\n\n\n', '\n2\nCalienta una sartén con rocío vegetal o 1 gotita de aceite desparramado con un papel o pincel de cocina. Luego, moja tus manos y toma 1 cucharada de la masa. Arma con ella una bolita del tamaño de una pelotita de golf.\n\n\n\n\n\n', '\n3\nAplasta la pelotita hasta obtener una arepa de 1,5 mm de ancho. Llévala a la sartén caliente y cocínala por aproximadamente 3 minutos o hasta que se despegue sola y veas que está ligeramente dorada. Repite este procedimiento con toda la masa.\n\n\n\n\n\n', '\n4\nDales la vuelta y cocínalas unos 3 minutos más. Sirve tus arepas paisa con tu platillo preferido, rellénalas con jamón y queso para un delicioso desayuno o guárdalas una vez frías en un recipiente hermético para consumirlas como snack.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepa paisa, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas colombianas.\n', '\nCon qué acompañar la arepa paisa\nAl igual que las arepas clásicas, las arepas paisas son muy versátiles. Para un rico y nutritivo desayuno, corta tu arepa paisa caliente por el medio y rellénala con jamón y queso. Caliéntala en el horno mientras preparas tu café con leche y cortas unas frutas, ¡empieza tu día con energía!También puedes preparar la clásica bandeja paisa, un típico y popular plato colombiano que combina:Frijoles antioqueños, cocidos con plátano verde, zanahoria, comino y cilantro.Arroz blanco.Carne molida y condimentada con comino, cebolla y ajo.Chorizo o morcilla.Plátanos fritos.Huevos fritos.Chicharrón,Salsa hogao, de cebolla, ajo y tomate.Aguacate.Y, por supuesto, las arepas paisa que haz aprendido a hacer en esta receta.Comparte esta deliciosa bandeja y sorprende a tus familiares y amigos con una típica bandeja paisa colombiana. Si pruebas las arepas o este platillo, nos encantaría que compartas con nosotros la foto del resultado en los comentarios. Descubre todos los tipos de arepas en este otro artículo. ¡A comer!\n', '\nFotos de Arepa paisa\n\n\n\n', '\nSube la foto de tu Receta de Arepa paisa\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1617,30 +1767,35 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-arepa-llanera-75492.html</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t>Receta de Arepa llanera</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n']</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar a preparar estas sencillas, pero deliciosas, arepas llaneras, calienta una sartén antiadherente con un poco de aceite. En ella, agrega la carne y baja el fuego a medio. Cocínala 7 minutos y dale la vuelta. Deja que se cocine otros 7 minutos más.\n\n\n\n\n\n', '\n2\nMientras se cocina la carne, lava y corta el tomate en cubos. Condiméntalo al gusto con el orégano o perejil fresco picado.\n\n\n\n\n\n', '\n3\nCalienta tus arepas y córtalas por el medio, pero sin llegar hasta el final. Debe quedarte como un libro, listas para rellenar. Prepara tus propias arepas con esta Receta de arepas de maíz fritas.Procede a armar tus arepas llaneras rellenando cada una con la carne con el tomate. Si lo deseas, puedes agregarle un aguacate cortado también en cubos. ¡A comer!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepa llanera, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nInformación nutricional de la arepa llanera\nEsta arepa es muy saludable y nutritiva. En 1 porción aporta 350 calorías. Además, al combinar hidratos, proteínas y vegetales, da mucha saciedad. Esto quiere decir que la comida estará por más tiempo en tu estómago, evitando que picotees a lo largo del día. Es por eso que si buscas bajar de peso o comer de forma saludable, esta opción es ideal para ti. Una vez más, comprobamos que comer saludable no es sinónimo de aburrido. ¡A disfrutar!Si pruebas esta receta, nos encantaría que compartas con nosotros la foto del resultado en los comentarios. Recuerda que puedes consultarnos cualquier duda\n', '\nSube la foto de tu Receta de Arepa llanera\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>15m</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1657,30 +1812,35 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-humitas-dulces-75476.html</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>Receta de Humitas dulces</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n']</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>['\n1\nPara empezar con la receta de humitas dulces primero debes desgranar el choclo, se puede utilizar con un cuchillo o con las manos limpias. No te olvides de reservar la coronta del maíz.\n\n\n\n\n\n', '\n2\nPasa por agua caliente la panca de maíz y resérvala.\n\n\n\n\n\n', '\n3\nLleva el maíz desgranado a una licuadora o a un triturador de alimentos.\n\n\n\n\n\n', '\n4\nIncorpora la leche y reserva.\n\n\n\n\n\n', '\n5\nEn una olla profunda derrite la mantequilla a fuego bajo.\n\n\n\n\n\n', '\n6\nUna vez se encuentre derretidala mantequilla añade el maíz licuado y mueve con la ayuda de una cuchara. Incorpora también el azúcar.\n\n\n\n\n\n', '\n7\nDespués de unos minutos incorpora la esencia de vainilla y el anís. Es importante no dejar de mover para evitar la formación de grumos.\n\n\n\n\n\n', '\n8\nAgrega las pasas y retira la olla del calor. Te darás cuenta de que la masa se encuentra lista cuando pases la cuchara y puedas ver el fondo de la olla.\n\n\n\n\n\n', '\n9\nCon la ayuda de una cucharada sirve en una panca de maíz.\n\n\n\n\n\n', '\n10\nEnvuelve la panca con mucho cuidado y dobla la punta de la panca hacia abajo.\n\n\n\n\n\n', '\n11\nColoca la humita encima de otra panca y envuelve nuevamente.\n\n\n\n\n\n', '\n12\nLa humita dulce debe quedar con la forma que observas en la imagen.\n\n\n\n\n\n', '\n13\nCierra las pancas con pabilo.\n\n\n\n\n\n', '\n14\nEn una olla grande agrega un chorro de agua y coloca las mazorcas de maíz formando una especie de cama.\n\n\n\n\n\n', '\n15\nColoca las pancas y las humitas. Es importante que las humitas no tengan contacto directo con el agua.\n\n\n\n\n\n', '\n16\nTapa y cocina aproximadamente 30-40 minutos.\n\n\n\n\n\n', '\n17\nRetira utilizando unas pinzas. ¡Listas para comer las humitas dulces!¿Qué te ha parecido esta receta de humitas de choclo dulces?\n\n\n\n\n\n', '\nSi te ha gustado la receta de Humitas dulces, te sugerimos que entres en nuestra categoría de Recetas de Tamales.\n', '\nValor nutricional de las humitas dulces\nEl maíz es el tercer cereal más consumido a nivel mundial. Es preferido por las personas celíacas, ya que no contiene gluten. Por cada 100 gramos de maíz se encuentran 86g de calorías, 19 g de carbohidratos, 1.2 g de grasas, 3.2g de proteínas y 270 gramos de potasio.Si eres amante de los platos peruanos y quieres conocer otras recetas, no te pierdas las siguientes elaboraciones:Pastel de chocloTarta de humitaEmpanadas de humita\n', '\nSube la foto de tu Receta de Humitas dulces\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>1h 30m</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1697,30 +1857,35 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-huaraches-de-pollo-75449.html</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>Receta de Huaraches de pollo</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n']</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>['\n1\nComienza la receta de huaraches de pollo preparando la masa, de manera que mezcla la harina de maíz con una pizca de sal y 1 taza de agua tibia hasta formar una masa. La masa debe quedar suave y ligeramente húmeda.\n\n\n\n\n\n', '\n2\nToma una porción de masa de unos 50 gramos, boléala y, con ayuda de un rodillo, extiéndela hasta que quede de unos 5 mm de grosor y haya tomado una forma ovalada.\n\n\n\n\n\n', '\n3\nEn un comal caliente, coloca el huarache y cocina cada lado de 2 a 3 minutos o hasta que se vea ligeramente tostado.\n\n\n\n\n\n', '\n4\nPara el guisado con pollo, en una olla con un poco de aceite, sofríe la cebolla y el jitomate picados. Luego, agrega el pollo en cubitos seguido por el chile serrano picado y cocina por unos 8 minutos o hasta que el pollo esté bien cocido.\n\n\n\n\n\n', '\n5\nColoca el huarache en un sartén o comal con un poco de aceite, unta un poco de frijoles refritos y agrega también nopales cocidos.\n\n\n\n\n\n', '\n6\nEnseguida, añade el guisado de pollo, un poco de queso rallado y salsa al gusto, ¡y listo! Ya puedes disfrutar de unos ricos huaraches de pollo con nopal.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Huaraches de pollo, te sugerimos que entres en nuestra categoría de Recetas de Antojitos mexicanos. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nHuaraches de pollo y otros ingredientes\nAnímate a preparar esta receta de huaraches de pollo, ya has visto que muy sencilla y en pocos pasos tendrás un rico antojito para disfrutar en familia. Utiliza como base la preparación del pollo de esta receta, aunque puedes dejar volar tu imaginación y hacer los cambios que quieras. Por ejemplo, en lugar de utilizar el pollo en cubos, puedes desmenuzarlo. Así mismo, puedes agregar al final alguna salsa de tomate verde, mole poblano o cualquier otra salsa que te guste.Como ves, hay bastantes combinaciones con las cuales puedes hacer los huaraches. Comparte con nosotros tu resultado y cuéntanos qué te pareció la receta.Si quieres conocer otra versión, no te pierdas la receta de huaraches de nopal.\n', '\nSube la foto de tu Receta de Huaraches de pollo\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>5 comensales</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1737,30 +1902,35 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tacos-de-coliflor-al-pastor-75438.html</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>Receta de Tacos de coliflor al pastor</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n']</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>['\n1\nPara hacer la receta de tacos de coliflor al pastor, en un recipiente agrega el jugo de naranja, el vinagre y el achiote. Mezcla para que se disuelva un poco el achiote y reserva.\n\n\n\n\n\n', '\n2\nEn un comal o sartén, asa el jitomate, el diente de ajo y el chile guajillo limpio. Dales vuelta a estos ingredientes para tatemarlos (asar) por todos sus lados. El chile guajillo no requiere de mucho tiempo, de manera que bastará con un par de minutos.\n\n\n\n\n\n', '\n3\nCuando el jitomate y el diente de ajo ya estén tatemados, pásalos a la licuadora con el chile guajillo, la mezcla de jugo de naranja y achiote, sal, pimienta al gusto y un clavo de olor. Licua todo durante unos 3 minutos y reserva.\n\n\n\n\n\n', '\n4\nEn una olla con un poquito de aceite, sofríe la cebolla morada hasta dorarla ligeramente. Luego, agrega la coliflor cocida y mueve constantemente por unos 3 minutos. Para cocinar la coliflor puedes hacerla en agua con sal o al vapor. No te pierdas nuestra receta de coliflor al vapor para conocer los tiempos exactos de cocción.\n\n\n\n\n\n', '\n5\nCuando la coliflor y la cebolla estén ligeramente doradas, agrega la salsa que licuaste, mezcla para integrar todos estos ingredientes y deja cocinar hasta que reduzca la salsa. Esto tomará alrededor de unos 8-10 minutos a fuego medio-bajo.\n\n\n\n\n\n', '\n6\nPara servir los tacos de coliflor al pastor, prepara tortillas de maíz y rellénalas. Luego, añade cilantro picado, piña asada al gusto y la salsa picante que más te guste.\n\n\n\n\n\n', '\n7\nEn este vídeo te enseñamos cómo hacer las tortillas de maíz para tus tacos de coliflor al pastor, ¡no te lo pierdas!\n\n\n\n', '\nSi te ha gustado la receta de Tacos de coliflor al pastor, te sugerimos que entres en nuestra categoría de Recetas de Tacos. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nCon qué acompañar los tacos de coliflor al pastor\n¿Qué te pareció esta versión de tacos al pastor? No te quedes sin probar esta receta, anímate a hacerla en casa para la cena o el almuerzo y comprueba que el sabor de estos tacos al pastor es muy similar al de los originales con carne de puerco. Lo mejor de todo de esta receta, ¡es que es ligera y baja en grasas! Ahora bien, si te apetece acompañar tus tacos de coliflor al pastor con una salsa picante, aunque esto implique aumentar un poco las calorías, te recomendamos las siguientes:Salsa para tacos al pastorSalsa machaSalsa de siete chiles\n', '\nSube la foto de tu Receta de Tacos de coliflor al pastor\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1777,30 +1947,35 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tinga-de-setas-75436.html</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>Receta de Tinga de setas</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n']</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>['\n1\nPara comenzar la receta de tinga de setas, prepara la salsa. Para ello, coloca en la licuadora los jitomates, el trozo de cebolla, el diente de ajo, chile chipotle adobado al gusto y un chorrito de agua. Licua muy bien y reserva.\n\n\n\n\n\n', '\n2\nEn una olla con un poco de aceite, sofríe la cebolla fileteada, moviéndola constantemente hasta que comience a ponerse transparente y se dore ligeramente.\n\n\n\n\n\n', '\n3\nCuando la cebolla esté lista, vierte la salsa que licuaste, sazona con sal, pimienta y una pizca de comino, mezcla y deja cocinar a fuego medio-bajo por 10 minutos.\n\n\n\n\n\n', '\n4\nMientras se cocina la salsa, corta en tiras las setas. Puedes usar un cuchillo o desmenuzarlas con tus manos. Resérvalas para seguir con la preparación de la tinga de setas.\n\n\n\n\n\n', '\n5\nPasados los 10 minutos de cocción de la salsa con la cebolla, agrega las setas cortadas en tiras, mezcla, comprueba el sabor y sazona un poco más si lo crees necesario. Deja cocinar hasta que las setas se hayan ablandado. Esto tomará alrededor de unos 5 minutos a fuego medio-bajo.\n\n\n\n\n\n', '\n6\n¡Y listo! Sirve esta deliciosa tinga de setas y acompáñala con unas ricas tostadas de maíz.\n\n\n\n\n\n', '\n7\n¡No te pierdas este vídeo para aprender a preparar tus propias tortillas de maíz!\n\n\n\n', '\nSi te ha gustado la receta de Tinga de setas, te sugerimos que entres en nuestra categoría de Recetas de Setas. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nCon qué acompañar la tinga de setas\nAnímate a preparar esta receta de tinga de setas, un platillo ideal si quieres un menú vegano para las próximas fiestas patrias. Puedes acompañarla con lechuga fresca, rábanos y frijoles en pasta. Si te gusta el picante, también puedes bañar tus tacos de tinga de setas con una salsa picosita, como estas:Salsa de cacahuate con chile de árbolSalsa macha\n', '\nSube la foto de tu Receta de Tinga de setas\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1817,30 +1992,35 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-tacos-de-barbacoa-75414.html</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>Receta de Tacos de barbacoa</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n']</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>['\n1\nComienza la receta de tacos de barbacoa cortando la carne de res. Puedes utilizar chambarete, falda o cualquier otro corte que se deshebre fácil.\n\n\n\n\n\n', '\n2\nEn una olla con 1 litro y medio de agua, agrega los dientes de ajo, las hojas de laurel, las pimientas negras enteras, una pizca de orégano seco, una pizca de tomillo, una pizca de mejorana, un trozo de cebolla, sal al gusto y, opcionalmente, chile quebrado seco. Deja que comience a hervir.\n\n\n\n\n\n', '\n3\nCuando esté hirviendo, agrega la carne de res, baja el fuego y deja que se cocine todo junto. El tiempo de cocción dependerá del tipo de olla, si utilizas olla de presión bastará con unos 30 minutos, mientras que si decides usar una olla convencional tomará alrededor de 2-3 horas, ya que necesitas que la carne esté suave y se deshebre fácilmente.\n\n\n\n\n\n', '\n4\nMientras se cocina la carne, pica finamente una cebolla mediana y una rama de cilantro. Reserva ambos ingredientes para seguir con la receta de tacos de barbacoa.\n\n\n\n\n\n', '\n5\nCuando la carne esté lista, retírala de la olla y deshébrala con ayuda de un tenedor o deja enfriar ligeramente y deshébrala con tus manos.\n\n\n\n\n\n', '\n6\nAhora solo queda armar los tacos de barbacoa, de manera que calienta la tortilla de maíz, agrega la barbacoa y, por último, añade cebolla y cilantro picados al gusto. No olvides añadir unas gotitas de limón y el toque picante con una buena salsa. Haz esta receta en casa, cuéntanos qué te pareció y si tienes algún ingrediente extra que le pongas, ¡a cocinar!¿Quieres preparar tu propia masa para tacos? ¡No te pierdas nuestra receta!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tacos de barbacoa, te sugerimos que entres en nuestra categoría de Recetas de Tacos. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTacos de barbacoa estilo Guadalajara\nPrepara esta receta donde quiera que vivas, puesto que los ingredientes son fáciles de conseguir en cualquier supermercado. Eso sí, lleva su tiempo, pero ten por seguro que al final tendrás un platillo de 10.Si quieres elevar el sabor de estos tacos de barbacoa, prueba haciéndolos fritos y acompañados con crema y queso, no te miento cuando te digo que así saben mucho mejor. Así mismo, puedes probar la versión de los tacos de barbacoa estilo Guadalajara, la cual se caracteriza por cocinar la carne enchilada. Para ello, con el mismo caldo de cocer la carne, puedes dejar en remojo chiles pasilla y chiles mirasol durante 10-15 minutos. Pasado este tiempo, puedes molerlos con 1-2 dientes de ajo, clavo, comino, pimienta entera, mejorana, ajonjolí 1 cucharadita de vinagre blanco y, si quieres, un trozo pequeño de jengibre. Esta mezcla añádela a la olla para acabar de cocinar la carne.Puedes acompañar estos tacos de barbacoa con otros tacos mexicanos, como estos:Tacos de huitlacocheTacos gobernador\n', '\nSube la foto de tu Receta de Tacos de barbacoa\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>4 comensales</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1857,22 +2037,27 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/articulo-tipos-de-arepas-75395.html</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>Tipos de arepas</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>['\nGeneralmente, las arepas se elaboran con harina de maíz o de trigo. Sin embargo, como veremos en el apartado correspondiente a las arepas colombianas, la masa puede variar considerablemente. Empezando por la recetas tradicionales, como decimos, distinguimos las siguientes:Arepas de harina de maízArepas de harina de trigoPor otro lado, actualmente encontramos toda una variedad que nos permite hacer arepas caseras originales, saludables y para todos los gustos. Por ejemplo, podemos hacer arepas con harina de avena, con remolacha e incluso con arroz. ¿Quieres saber cómo preparar estas arepas? ¡Aquí tienes las recetas!Arepas de cocoArepas de remolachaArepas de avenaArepas de arroz sin harinaArepas de plátano verdeArepas de batataArepas de chíaArepas de auyamaArepas de papaArepas de zanahoriaComo ves, existen un sinfín de recetas de arepas para elaborar la masa, ahora bien, ¿de qué rellenarlas? A continuación, mostramos los tipos de arepas venezolanas y colombianas más habituales.\n', '\nClasificar los diferentes tipos de arepas provenientes de Venezuela no resulta una tarea nada fácil, pues no existe aún un registro fiable que las reúna a todas, por eso resulta difícil precisar cuántas existen, aunque hay quienes dicen que están entre 40 y 80 variedades.Por todo lo dicho anteriormente, solo nos concentraremos en las principales arepas rellenas, pues estas definen mucho el estilo venezolano. Es interesante mencionar que, si comes una arepa en un local de comida en Venezuela, puedes pedirla mixta (una arepa personalizada) y agregarle encima salsas al gusto, comúnmente guasacaca o picante. Dicho esto, veamos cómo se clasifican algunas arepas venezolanas:Reina pepiada. El relleno consiste en una crema preparada con carne mechada de pollo o gallina, aguacate triturado, mayonesa o yogur griego. Además, se le agrega tajadas de aguacate.Sifrina. Tiene el mismo contenido que la reina pepiada, pero adicionalmente contiene queso amarillo.Peluda o pelúa. Consiste en carne de res mechada o deshebrada (tinga de res) y queso blanco rallado.Catira. Contiene pollo deshebrado y queso rallado.Dominó. Este tipo de arepa venezolano se le llama así por la combinación de colores que proporcionan sus ingredientes de relleno, caraotas negras y queso blanco, los cuales nos recuerdan a las piezas de ese juego tan famoso.Pabellón criollo. Esta arepa tiene los ingredientes típicos del platillo icónico de las gastronomía venezolana: carne de res mechada, tajadas (plátano macho frito), queso blanco rallado y caraotas negras (frijoles negros).Llanera. Esta arepa venezolana está rellena de carne asada cortada en tiras, aguacate en tajadas, tomate en rodajas y queso guayanés o queso blanco rallado.Gringa o musiúa. Se le llama así porque sus ingredientes son los mismos que los empleados para una hamburguesa tradicional (carne, vegetales y salsas), aunque se sustituye el pan por una arepa.Santa Bárbara. Contiene un bistec de carne de res acompañado con queso y aguacate.Rumbera. Consiste en una arepa rellena con pernil y queso rallado.Tumbarranchos. Para esta preparación se emplea una arepa del día anterior (conocidas como tostadas), la cual se rellena con mortadela y se fríe. Además, se acompaña con salsas, quesos, carnes y verduras.Rompe colchón. Este delicioso tipo de arepa esté lleno con una mezcla de mariscos.A caballo. Así se denomina cuando la arepa tiene encima un huevo frito.Arepa endiablada. El relleno consiste en carne de cerdo molida y enlatada. Se le dice endiablada por una marca famosa.Perico. Esta arepa se rellena con un revoltillo de huevos con tomate, cebolla y ají dulce.Arepa con queso. Hay una gran variedad, pues en Venezuela existe una amplia gama de quesos, mayormente del tipo fresco. Las arepas más populares en esta reglón son las de queso amarillo, queso guayanés o queso telita. Además, a esta combinación se le puede agregar mantequilla o no, y el queso se usa rallado o en una pieza gruesa.Arepa con jamón y queso. Contiene jamón cocido, queso mozzarella o gouda. Algunas personas también le agregan huevo cocido.Arepa con tajada. Este antojito muestra el típico sabor venezolano salado-dulce, con una combinación de tajadas (plátano macho maduro) con queso blanco fresco.Arepa con huevos de codorniz. Los huevos de codorniz se mezclan con salsa rosada antes de agregarlos a la arepa.Arepa con raya. Consiste en carne mechada o deshebrada de raya guisada.Arepa con cazón. El contenido se prepara igual que la raya, tipo carne mechada.Arepa con atún. El relleno de esta arepa consiste en una mezcla de atún, tomate, cebolla y mayonesa.Arepa con ensalada de pernil. Lleva rebanadas de carne de cerdo horneado, rodajas de tomate y mayonesa. Después del 24 de diciembre, en los hogares venezolanos suele ser una receta de aprovechamiento, pues los restos de pernil de la cena sirven de relleno para estas arepas.Arepa con ensalada de gallina. La ensalada puede ser simple (mayonesa, papas, y zanahorias) o la receta completa usada en Navidad. Esta preparación en diciembre, en muchos hogares venezolanos, también se usa como receta de aprovechamiento del “día después”.Otras arepas venezolanas rellenas tradicionales: carne mechada (a veces le agregan queso), carne molida, asado negro, con vísceras (hígado y molleja, etc.), con embutidos (chorizo, salchicha o mortadela, mezclados con una salsa), pollo deshebrado guisado, etc.Arepas gourmet: rellenas con cordero, salmón rojo, camarones y aguacate, etc.\n\n\n\n\n\n\n\n\n', '\nAl igual que pasa con las arepas venezolanas, no hay una clasificación establecida que sirva de guía definitiva, pero se presume que pueden existir entre 40 y 80 tipos de arepas colombianas. Es interesante mencionar que entre las arepas colombianas y las venezolanas hay muchas similitudes, como a continuación podrás verificar, sin embargo, también existen importantes diferencias que definen la identidad de cada lugar. Dicho esto, te invitamos a explorar las variedades colombianas de esta deliciosa expresión culinaria latinoamericana:Arepa de choclo. La arepa de choclo se preparar a partir de granos de maíz tierno, leche, azúcar y sal. Así, se obtiene un producto semejante a un panqueque, pues su textura es esponjosa y su sabor algo dulce. Esta preparación se rellena con queso campesino y es hermana de la cachapa venezolana, la cual es idéntica, pero se rellena de formas más diversas, aunque en Venezuela muchos no la consideran propiamente una arepa.Arepa boyacense. Este aperitivo destaca por su sabor peculiar, que mezcla lo dulce y lo salado, característica que hace que se asemeje mucho a algunas clases de arepas venezolanas. Para elaborar la arepa boyacense se prepara una masa con maíz precocido, harina de trigo, panela, sal y cuajada, posteriormente se le da forma y se cocina en una parrilla u horno de barro. Sirve de acompañamiento tanto en almuerzos con carnes como en desayunos.Arepa paisa. Esta arepa de maíz trillado se caracteriza por dos cosas: no contiene relleno y su grosor es muy delgado. Una vez lista, se sirve untándola por encima con mantequilla y, posteriormente, cubriéndola con queso blanco. También funciona como acompañante de comidas como el chorizo.Arepa valluna. La arepa valluna y la arepa paisa prácticamente son lo mismo, aunque se diferencian principalmente en dos cosas: el grosor y el momento en que se le agregan los acompañantes. La valluna es más gruesa que la paisa, suele cocinarse sobre una parrilla de alambre y, justo a mitad de cocción, se le agrega la mantequilla y el queso rallado.Arepa costeña o arepa de huevo. Consiste en una arepa hecha con maíz amarillo, la cual se precocina en aceite, después se le hace un orificio, se le agrega el huevo crudo y se fríe de nuevo. En Venezuela, específicamente en el estado Zulia, también se prepara este tipo de arepa.Arepa de chicharrón o arepa santandereana. Este aperitivo consiste en una masa preparada con los siguientes ingredientes molidos: maíz preferiblemente amarillo (pelado y cocido), chicharrón de cerdo y yuca cocinada. Una vez lista la masa, se le da forma de arepa y se cocina sobre una plancha que tenga cenizas disueltas en agua (el toque secreto de esta preparación). Se sirve comúnmente como acompañante de sopas y huevos revueltos. En Venezuela también hay arepa de chicharrón, pero la preparación puede variar dependiendo de la región.Arepa rellena. La arepa rellena también está presente en la gastronomía colombiana, aunque de forma más puntual y no tan habitual como en Venezuela. Los rellenos más comunes son carne, pollo, tocino, aguacate, plátano maduro y chorizo. Algunas veces, acompañados con cebolla, pimentón y cilantro.\n\n\n\n\n\n\n\n\n', '\nAunque los principales exponentes de la arepa son Venezuela y Colombia, este alimento también forma parte del acervo culinario de muchos otros países, en algunos debido a intercambios culturales y en otros debido a su patrimonio cultural indígena. Por eso, a continuación, reunimos los más reconocidos, aunque muy probablemente existan muchos otros tipos de arepas:Arepa canaria. La arepa canaria es idéntica a la arepa venezolana y surge como producto de una conexión muy especial entre ambos lugares (especialmente Tenerife), debido a las emigraciones sucedidas en diferentes épocas hasta el presente y los consecuentes intercambios culturales. En los bares y restaurantes de las islas suelen prepararlas fritas y, muchas veces, les incorporan ingredientes de la gastronomía local, como el queso tierno o el plátano canario.Tortilla o arepa panameña. Se trata de una masa de maíz viejo a la que, dependiendo del gusto, se le puede agregar plátano o queso rallado para después cocinarla asada o frita. También tienen otra variante llamada changa o tortilla changa, preparada con maíz nuevo, la cual se caracteriza por su gran tamaño. Este tipo de arepa se asemeja mucho a la arepa venezolana y colombiana.Pupusas. La pupusa es muy semejante a una arepa gruesa y está hecha con masa de maíz o de arroz. Comúnmente se rellena con una gran variedad de ingredientes, especialmente de tipo local. Se dice que podría tener su origen en la cultura maya quiché. Esta comida se consume en Guatemala, Honduras y El Salvador. Los rellenos habituales son flor de loroco, cochinito, pitos, hojas de chipilín, hierba mora, espinacas, ayote, jamón, carne de pollo o res, etc.Gorditas. Aunque las gorditas no son reconocidas como arepas, tienen todas las características de estas. Se trata de una tortillas de maíz o trigo que se preparan en formas diversas: se rellenan antes de cocerlas, se abren para rellenarlas después de cocidas o se sirven con el relleno por encima. Este antojito mexicano se cocina frito o directo en el comal y puede ser dulce o salado. Es interesante mencionar que en Yucatán existe una galleta espolvoreada con azúcar y preparada con harina de maíz llamada arepa.Arepas puertorriqueñas. Este tipo de aperitivo es muy parecido a la arepa andina venezolana preparada con trigo. Ambas se pueden comer dulces o saladas.Arepa cubana. Aunque se llama así, en Cuba se refieren realmente a un panqueque (crepe o tortita), preparado al estilo tradicional. Algo parecido sucede con la tica o arepa costarricense.Por último, aunque la arepa no es nativa del Perú, ahora la degustan allí, incluso con rellenos autóctonos.\n', '\nSi te ha gustado el artículo Tipos de arepas, te sugerimos que entres en nuestra categoría de Arepas.\n']</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1885,30 +2070,35 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-molotes-poblanos-75413.html</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>Receta de Molotes poblanos</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n']</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t>['\n1\nPara hacer la receta de molotes poblanos, primero prepara la masa de maíz. Para ello mezcla la harina de maíz nixtamalizado, la sal, el polvo para hornear y la harina de trigo. Luego, agrega poco a poco agua tibia hasta formar la masa, también puedes agregar un poco de aceite o manteca. Cubre con un paño húmedo y deja reposar.\n\n\n\n\n\n', '\n2\nMientras reposa la masa prepara la tinga de pollo. En una olla con un poco de aceite fríe la cebolla en juliana y sazona con un poco de sal y pimienta.\n\n\n\n\n\n', '\n3\nAgrega el puré de tomate y mezcla muy bien. Enseguida agrega el pollo desmenuzado y mezcla una vez más, comprueba el sabor y si es necesario agrega un poco más de sal. Reserva.\n\n\n\n\n\n', '\n4\nCon la masa reposada es momento de preparar los molotes de pollo. Toma una porción de masa y boléala ligeramente.\n\n\n\n\n\n', '\n5\nUtiliza una prensa para las tortillas y presiona la masa ligeramente. Procede a rellenar los molotes poblanos con la tinga de pollo.\n\n\n\n\n\n', '\n6\nCierra por los lados para cubrir el relleno de los molotes, si se abre añade con un poco más de masa o acomoda los bordes presionando.\n\n\n\n\n\n', '\n7\nFríe en un sartén u olla con suficiente aceite hasta que estén dorados, después retira del aceite y coloca sobre papel absorbente.\n\n\n\n\n\n', '\n8\nPara servir, acompaña con crema y salsa de tu preferencia. Listo, ya puedes disfrutar de unos ricos y crujientes molotes poblanos. ¡A comer!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Molotes poblanos, te sugerimos que entres en nuestra categoría de Recetas de Antojitos mexicanos. También puedes visitar una selección de las mejores recetas mexicanas y recetas poblanas.\n', '\nMolotes poblanos, un gran platillo tradicional\nDesde la época colonial y con la llegada de los españoles, se introdujeron nuevos elementos a la cocina prehispánica y con ello, muchos platillos han adoptado un sabor excepcional, los molotes poblanos son un claro ejemplo y es que la preparación de estos ha variado con el tiempo y cada vez hay recetas de rellenos. Señalamos que existe una feria del molote que se realiza anualmente en Cholula Puebla, en esta ciudad se pueden encontrar diferentes tipos de molotes y están exquisitos. ¡Prepara esta receta y prueba el rico sabor tradicional poblano!Y si además, quieres conocer más recetas mexicanas, no te pierdas estas recetas:Molotes veracruzanosMolotes de OaxacaMolotes de plátano con quesoQuesadillas de pollo mexicanasQuesadillas fritas de papas\n', '\nSube la foto de tu Receta de Molotes poblanos\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>6 comensales</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>45m</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1925,30 +2115,35 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-gyros-griego-75396.html</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>Receta de Gyros griego</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar fundido. Enciende el horno para que se caliente a temperatura máxima, 200 ºC. ¿Qué te están pareciendo estas hamburguesas con tapa de empanadas?\n\n\n\n\n\n', '\n6\nAgrega la carne y cierra el disco. Puedes hacer el clásico repulgue, cerrarla hacia adelante como una medialuna o con la ayuda de un tenedor.\n\n\n\n\n\n', '\n7\nDispón las empanadas en una asadera con un poco de aceite o rocío vegetal. Sepáralas 2-3 centímetros para que se cocinen de forma pareja y píntalas con el huevo batido. Además, también puedes decóralas con las semillas de sésamo, como el pan clásico de las hamburguesas. Cocínalas en el horno a 200 ºC aproximadamente 15-20 minutos o hasta que la masa esté dorada. ¡Ya puedes comer las hamburguesas envueltas en masa de empanadas!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Empanadas de hamburguesa, te sugerimos que entres en nuestra categoría de Recetas de Empanadas.\n', '\nEmpanadas de hamburguesa al horno\nPara que la cocción al horno sea saludable, debes utilizar poco aceite. Para ello, toma 1 cucharadita de aceite y vuélcala sobre la asadera. Con la ayuda de las manos o de una servilleta, distribúyela a lo largo y ancho de la asadera. Por el contrario, si añades aceite sin medir y este cubre una parte de la empanada, lo absorberá durante la cocción y sus calorías serán incluso más altas que si realizas una fritura saludable con abundante aceite.El disco de empanada está compuesto por harina de trigo que, al cocinarla en fritura, absorbe un 15% del peso del alimento de aceite. Esto representa unas 135 calorías cada 100 gramos, aproximadamente el peso de la mitad de una empanada. Sabiendo que el alto consumo de grasas está relacionado con enfermedades cardiometabólicas como la hipercolesterolemia, diabetes e hipertensión, recomendamos que pruebes esta cocción al horno, pues casi no existe absorción de aceite.Y, si eres un amante de las empanadas, te ofrecemos otras recetas deliciosas:Empanadas de champiñonesEmpanadas de humitaEmpanadas de jurelEmpanadas de atún\n', '\nSube la foto de tu Receta de Empanadas de hamburguesa\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de torre de panqueques salada fría, primero debes armar los panqueques. Para ello, hidrata la harina con el huevo y la leche en la heladera aproximadamente 20 minutos. Mientras, cocina los huevos con abundante agua fría por 12 minutos. Pasados los 20 minutos de hidratación de la harina, cocina los panqueques en una sartén con rocío vegetal o con 1 cucharadita de aceite con una servilleta. Cuando esté caliente, baja el fuego a medio y agrega 1 cucharón de la preparación. Cuando empiecen las burbujas, dale la vuelta con cuidado y cocínalo por el otro lado hasta que se hagan burbujas. Repite el proceso con el resto de la masa y reserva en la heladera para que se enfríen.\n\n\n\n\n\n', '\n2\nEmpieza el armado de la torta de panqueques salada untando 1 panqueque con 1 cucharada de mayonesa y añadiendo en la parte superior las hojas verdes cortadas. Unta el siguiente panqueque y dispón mayonesa sobre las hojas para que no se muevan. Luego, unta el otro lado del panqueque y agrega las fetas de queso.\n\n\n\n\n\n', '\n3\nAgrega un panqueque más, úntalo con mayonesa y dispón el tomate cortado en rodajas finas.\n\n\n\n\n\n', '\n4\nA continuación, unta otro panqueque con la mayonesa y añade encima más hojas verdes cortadas. Unta el siguiente panqueque y disponlo con la mayonesa sobre las hojas para que no se mueva. Unta el otro lado del panqueque y agrega las fetas de jamón natural.\n\n\n\n\n\n', '\n5\nColoca el último panqueque y úntalo con mayonesa. Por último, decora tu torre con el huevo duro picado. Déjalo enfriar 15-20 minutos en congelador tapado o 2 horas en heladera. Su sabor será aún más rico si lo haces de un día para otro. Sírvelo como entrante o como plato principal con una abundante ensalada. Disfruta de esta torta salada de panqueques y cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torre de panqueques salada, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nOtros rellenos para la torre de panqueques salada\nAdemás de esta opción que compartimos contigo, puedes rellenar esta torre de fiambre con diferentes ingredientes, como por ejemplo: pollo desmenuzado con mayonesa, atún natural, zanahoria rallada, palmitos, palta, pepino en rodajas y remolacha rallada. Y, si quieres hacer una torre de panqueques salada light o una torre de panqueques vegetariana, puedes escoger ingredientes saludables y con un contenido bajo en calorías. Elige el relleno que más te guste o los ingredientes que tengas en casa para disfrutar esta Navidad de una fresca y rica torre de panqueques.¿Te gustaría conocer más recetas de panqueques? No te pierdas estas opciones:Panqueques sin huevoPanqueques sin lechePanqueques de plátanoPanqueques de quinoa\n', '\nSube la foto de tu Receta de Torre de panqueques salada\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de calabaza, primero debes limpiar muy bien las hojas para hacer el tamal y dejarlas remojar en agua caliente por un mínimo de 20 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nEn un bol mezcla la leche caliente, el piloncillo, el clavo de olor, la nuez moscada y la canela en polvo.\n\n\n\n\n\n', '\n3\nAgrega la harina de maíz y la manteca vegetal, mezcla manualmente o con la ayuda de una batidora.\n\n\n\n\n\n', '\n4\nAgrega el puré de calabaza y el polvo para hornear, mezcla todo muy bien hasta integrar por completo.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Primero toma una de las hojas de maíz, extiende con tus manos y agrega una porción de masa, extiende de centro hacia arriba, envuelve y cierra bien. Señalamos que puedes atarlo con tiras de hojas o dejarlo solo doblado. Con las cantidades mencionadas pueden salir aproximadamente entre 20-25 tamales dependiendo del tamaño. Acomoda los tamales de forma vertical en una olla vaporera, cubre con una bolsa plástica o con algunas hojas que te hayan sobrado y cocina a fuego medio bajo aproximadamente una hora. ¡Ya casi están los tamales de calabaza mexicanos!\n\n\n\n\n\n', '\n6\nCuando estén listos, la hoja se desprenderá fácilmente y ya podrás degustar los deliciosos tamales de calabaza dulce. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de calabaza, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nOtros ingredientes para elaborar tamales de calabaza\nPreparar tamales es muy sencillo y una vez aprendes a hacerlos, solo basta con variar el relleno o el sabor que más te guste. Además de los ingredientes que te presentamos en esta receta, puedes incluir más en el relleno o en la masa, como por ejemplo: nueces, queso crema o dulce de leche, este en especial queda muy bien con el sabor de la calabaza.Por otra parte, dependiendo la región donde se cocinen los tamales, se pueden encontrar otras formas de incluir la calabaza en los tamales, por ejemplo: se pueden preparar también tamales salados de calabaza con un adobo de chiles guajillo y un toque de camarón seco, estos se envuelven en hoja de plátano. Además de estos ingredientes, señalamos que nuestros preferidos son los tamales de calabaza y frijol y los tamales de camarón. ¡Están deliciosos!Si te gustan las recetas de tamales y quieres conocer diferentes combinaciones, sigue leyendo:Tamales de acelgaTamales de dulceTamales de frijolesTamales de Nutella\n', '\nSube la foto de tu Receta de Tamales de calabaza\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de Nutella, primero debes remojar las hojas para tamal en agua caliente aproximadamente unos 30 minutos para que se suavicen.\n\n\n\n\n\n', '\n2\nPara hacer la masa de los tamales de Nutella, en un recipiente mezcla la masa de maíz, el polvo para hornear y la manteca vegetal.\n\n\n\n\n\n', '\n3\nAgrega la leche condensada y poco a poco la leche tibia, mezcla nuevamente para ir integrando todos los ingredientes.\n\n\n\n\n\n', '\n4\nPara terminar la masa, agrega la Nutella y una pizca de sal, mezcla una última vez hasta obtener una textura suave, ligera y húmeda.\n\n\n\n\n\n', '\n5\nCon la masa lista, es momento de armar los tamales. Escoge una hoja de tamal, extiende con tus manos y agrega una porción de masa, distribuye bien por la hoja sin llegar a las puntas, envuelve y cierra bien, acomoda en una olla vaporera. Con las cantidades mencionadas en la receta pueden salir 20-25 tamales dependiendo del tamaño.\n\n\n\n\n\n', '\n6\nSi te sobraron algunas hojas de tamal, cubre los tamales en la olla con las mismas hojas o bien con un trapo húmedo o una bolsa plástica, cocina aproximadamente 1 hora. ¿Qué te está pareciendo esta receta de tamales rellenos de Nutella?\n\n\n\n\n\n', '\n7\nPasado el tiempo de cocción, deja enfriar un poco y sirve estos ricos tamales dulces de chocolate. Cuéntanos en los comentarios qué te ha parecido esta receta mexicana. Para los amantes del chocolate seguro que será la receta favorita para comer durante las próximas fiestas.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de Nutella, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales dulces de Nutella y otros toppings\nComo has podido ver en esta receta, se agregó la Nutella a la masa, pero puedes dejar la masa sin la Nutella y agregarla como relleno. Además, puedes incorporar con algunas chispas de chocolate o con trozos de chocolate con avellanas. También señalamos que los tamales de Nutella y oreo están deliciosos. ¡Escoge el topping que más te guste! Es cierto que tal vez pienses que es mucho azúcar entre la Nutella y la leche condensada, sin embargo, para los tamales dulces se recomienda que tenga dulzor extra, pues al momento de cocinarlos en la vaporera el mismo dulzor a causa del vapor se reduce considerablemente. Sin embargo, procura disfrutar con moderación de estos tamales.Si quieres conocer más recetas de tamales dulces, no te pierdas estas recetas fáciles y deliciosas:Tamales de dulceTamales canariosTamales de elote dulcesTamales de chocolate y nuez\n', '\nSube la foto de tu Receta de Tamales de Nutella\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara hacer la receta de tamales de frijoles primero debes remojar en agua caliente las hojas para hacer el tamal, aproximadamente unos 20 o 30 minutos para que se suavicen y sea más fácil manipularlas.\n\n\n\n\n\n', '\n2\nEn un recipiente coloca la masa de maíz, la manteca que puede ser vegetal o de cerdo, las hojas de epazote finamente picadas y la pizca de sal, mezcla muy bien.\n\n\n\n\n\n', '\n3\nColoca en la licuadora los frijoles cocidos con un trozo de cebolla y licua hasta obtener una pasta de frijoles. Seguido, reserva.\n\n\n\n\n\n', '\n4\nEn una superficie limpia extiende la masa de maíz hasta obtener un grosor de unos 3 milímetros, señalamos que puedes hacerlo con tus manos o con un rodillo.\n\n\n\n\n\n', '\n5\nEnseguida agrega la pasta de frijol y distribuye por toda la masa a modo de capa.\n\n\n\n\n\n', '\n6\nEnrolla la masa con la pasta y luego corta en porciones de unos 8 cm de largo. Bolea conservando la forma del rollo. ¿Qué te está pareciendo este tamal de frijol negro?\n\n\n\n\n\n', '\n7\nColoca la masa enrollada en una hoja de maíz, envuelve, enrosca las puntas y presiona hacia dentro del relleno. Debe quedar como si se escondieran las puntas, luego lleva a una olla vaporera y cocina aproximadamente una hora. Señalamos que los tamales de frijol en hoja de milpa están también deliciosos.\n\n\n\n\n\n', '\n8\nPasado el tiempo de cocción, verifica que la hoja de maíz se desprenda fácil del tamal, si es así, ya estarán listos. Señalamos que existen diferentes versiones para elaborar tamales, destacamos que los tamales de frijoles hondureños y los tamales de frijoles veracruzanos, son también muy populares. Disfruta de esta receta y cuéntanos en los comentarios qué te ha parecido esta elaboración. Además, también puedes acompañarlos con mole poblano y queso fresco. Y si te gusta el picante, puedes preparar un delicioso mole verde.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de frijoles, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de frijol dulce\nSi eres más de sabores dulces, a continuación te proporcionamos una breve explicación para que conviertas estos tamales de frijoles mexicanos en una elaboración dulce. El proceso de la masa es el mismo, solo que deberás omitir el epazote. Pues bien, cuando tengas tu masa lista, reserva y prepara el relleno: licua los frijoles con una cucharadita de canela y unos 3 clavos de olor, mezcla con 500 g de piloncillo rallado hasta formar una pasta ligera. Para armar los tamales, extiende una hoja, agrega una porción de masa y extiende también, enseguida agrega una porción de la pasta de frijol con piloncillo, envuelve y cierra bien. En cuanto al método de cocción, este es el mismo.Y, si quieres conocer otras recetas de tamales, sigue leyendo:Tamales de rajasTamales canariosTamales de dulce\n', '\nSube la foto de tu Receta de Tamales de frijoles\n\n\n\nSube la foto de tu plato \n\n\n', '\nConvertido en icono gastronómico europeo, el Jamón Ibérico ha traspasado los límites de la gastronom</t>
+          <t>['\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n']</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>['\n1\nPara hacer la receta de gyros griego, primero prepara la salsa tzatziki. Para ello, ralla el pepino y luego drena el agua con ayuda de un colador. Este líquido puedes usarlo para preparar un jugo verde. \n\n\n\n\n\n', '\n2\nMezcla el pepino colado con el yogur, el ajo en pasta, el eneldo, el aceite de oliva, el jugo de limón y sal y pimienta al gusto. Reserva la salsa para seguir con la receta de gyros.\n\n\n\n\n\n', '\n3\nPrepara el pollo, de manera que calienta un poco de aceite en una sartén u olla. Cuando esté caliente, cocina el pollo sazonando con un poco de sal, pimienta y ajo en polvo, mezcla para integrar los sabores y cocina durante 3 minutos.\n\n\n\n\n\n', '\n4\nAgrega el jugo de limón y el orégano seco, mezcla y cocina por 3 minutos más.\n\n\n\n\n\n', '\n5\nPara terminar de cocinar el pollo, agrega la mostaza, mezcla una última vez y cocina por 5 minutos más. Recuerda que puedes utilizar carne de cerdo o de cordero para preparar tu gyros griego, ya que el proceso es el mismo. \n\n\n\n\n\n', '\n6\nCuando el pollo esté listo, retíralo del fuego y córtalo como más te guste para facilitar el posterior montaje del gyros. Nosotros hemos optado por cortarlo en tiras.\n\n\n\n\n\n', '\n7\nAhora es momento de armar el gyros. Primero, calienta el pan de pita en una sartén hasta que lo notes suave. Luego, colócalo sobre un plato, agrega una cucharada de la salsa tzatziki y distribúyela por todo el pan.¿Quieres aprender a preparar tu propio pan? En RecetasGratis tenemos la Receta de pan de pita.\n\n\n\n\n\n', '\n8\nEnseguida, agrega el pollo cocinado, la cebolla cortada en juliana, las rebanadas de tomate y la lechuga al gusto.\n\n\n\n\n\n', '\n9\nEnrolla con un trozo de papel de aluminio o papel encerado y estará listo para llevar y comer. Aunque pueda parecer un proceso largo, lo cierto es que preparar gyros de pollo no es tan complicado. Anímate a probarlo y cuéntanos qué te ha parecido.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Gyros griego, te sugerimos que entres en nuestra categoría de Recetas de Wraps.\n', '\nCon qué acompañar el gyros griego\nEsta es una receta sencilla y llena de sabor y sazón que estamos seguros te va a encantar. Como mencionamos al inicio de la receta, puedes elegir rellenar tu gyros griego con pollo, cerdo o cordero, incluso hay algunas recetas vegetarianas que son igual de ricas. Para el gyros de cerdo, recomendamos utilizar lomo.Los gyros griegos han traspasado fronteras y se han vuelto muy populares como comida rápida en diferentes partes del mundo. Además, cada lugar le ha dado su toque de sabor. En cuanto a sus acompañamientos, puedes disfrutar de este delicioso plato con una sencilla ensalada griega y con patatas fritas.Anímate a preparar este rico platillo, explora nuevas combinaciones y disfruta de este rico sándwich en rollo que puedes llevar prácticamente a todos lados.\n', '\nSube la foto de tu Receta de Gyros griego\n\n\n\nSube la foto de tu plato \n\n\n']</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>5 comensales</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>30m</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>Dificultad baja</t>
         </is>
@@ -1965,30 +2160,35 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>https://www.recetasgratis.net/receta-de-molotes-veracruzanos-75386.html</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>Receta de Molotes veracruzanos</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>['\n\n\n12 champiñones\n\n', '\n\n\n1 pimiento verde\n\n', '\n\n\n1 pimiento rojo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 puñado de queso rallado \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 puñado de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n9 aceitunas verdes sin hueso\n\n', '\n\n\n10 gramos de queso fresco \n', '\n\n\n1 huevo\n\n', '\n\n\n30 gramos de pan rallado \n', '\n\n\n20 gramos de harina \n', '\n\n\n1 cucharadita de aceite \n', '\nPara hacer la masa de crepas\n', '\n\n\n300 gramos de harina de maíz blanco precocida/Harina de maíz amarillo precocida \n', '\n\n\n470 mililitros de agua \n', '\n\n\n4 gramos de sal \n', '\nPara el relleno de manzana y queso de cabra\n', '\n\n\nqueso feta\n\n', '\n\n\nrúcula\n\n', '\n\n\ncanónigos\n\n', '\n\n\n3 nueces\n\n', '\n\n\n1 manzana\n\n', '\n\n\n1 cebolla\n\n', '\n\n\nazúcar moreno\n\n', '\n\n\naceite de oliva\n\n', '\n\n\nvinagre balsámico de Módena\n\n', '\npara el relleno de guisantes y calabacín\n', '\n\n\n1 tomate pera maduro\n\n', '\n\n\n1 pimiento amarillo\n\n', '\n\n\n1 lima\n\n', '\n\n\n200 gramos de guisantes \n', '\n\n\n1 calabacín\n\n', '\n\n\n1 pizca de pimienta negra \n', '\n\n\n1 cucharada sopera de cebollino fresco picado \n', '\n\n\n1 cucharada sopera de perejil fresco picado \n', '\n\n\n1 diente de ajo \n', '\n\n\n125 gramos de mozzarella (1 bola fresca) \n', '\n\n\n50 gramos de almendra molida \n', '\n\n\n2 cucharadas soperas de queso crema \n', '\n\n\n2 cucharadas de postre de ajo en polvo \n', '\n\n\n1 pizca de levadura química \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de queso parmesano rallado \n', '\n\n\n2 cucharadas soperas de aceite de oliva \n', '\n\n\n1 zanahoria mediana\n\n', '\n\n\n1 coliflor mediana\n\n', '\n\n\n1 pimiento rojo mediano\n\n', '\n\n\n2 ramas de cebolla china o cebollin \n', '\n\n\n1 cebolla blanca mediana\n\n', '\n\n\n4 huevos\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimiento \n', '\n\n\n1 rama de perejil \n', '\n\n\n400 gramos de harina de maíz nixtamalizada \n', '\n\n\n2½ tazas de agua tibia \n', '\n\n\n½ taza de azúcar (100 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 cucharón de vainilla \n', '\n\n\n1 cucharadita de canela en polvo \n', '\n\n\n400 gramos de piña en trozo \n', '\n\n\n200 gramos de coco rallado (2 tazas)\n\n', '\n\n\n1 taza de almíbar o jugo de piña \n', '\n\n\n90 gramos de mantequilla derretida \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n20 discos de empanada\n\n', '\n\n\n500 gramos de carne picada \n', '\n\n\n250 gramos de cebolla \n', '\n\n\n50 gramos de queso cheddar fundido \n', '\n\n\n1 cucharada postre de pimentón ahumado \n', '\n\n\n½ cucharada postre de comino \n', '\n\n\n¼ cucharada postre de ají molido \n', '\n\n\n1 huevo\n\n', '\n\n\n1 cucharada sopera de semillas de sésamo blanco \n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\n25 centímetros cúbicos de vino tinto \n', '\nPara los panqueques\n', '\n\n\n1 huevo\n\n', '\n\n\n100 gramos de harina 000 \n', '\n\n\n200 centímetros cúbicos de leche \n', '\nPara las capas:\n', '\n\n\n2 láminas de jamón natural \n', '\n\n\n2 láminas de queso en fetas \n', '\n\n\n1 tomate\n\n', '\n\n\n50 gramos de lechuga, espinaca y rúcula \n', '\n\n\n2 huevos\n\n', '\n\n\n6 cucharadas soperas de mayonesa \n', '\n\n\n400 gramos de harina para tamales \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n100 gramos de piloncillo rallado o en cono \n', '\n\n\n2 tazas de leche caliente \n', '\n\n\n1½ tazas de puré de calabaza \n', '\n\n\n1 cucharadita de canela molida \n', '\n\n\n1 cucharadita de clavo de olor en polvo \n', '\n\n\n1 cucharadita de nuez moscada \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n30 hojas de para tamales \n', '\n\n\n500 gramos de masa de maíz \n', '\n\n\n½ taza de leche condensada (120 gramos)\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1½ tazas de leche tibia \n', '\n\n\n400 gramos de nutellla o dulce de avellanas \n', '\n\n\n1 pizca de sal \n', '\n\n\n200 gramos de manteca vegetal o mantequilla \n', '\n\n\n30 hojas de para tamal \n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n150 gramos de manteca vegetal o de cerdo \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de frijol cocido \n', '\n\n\n3 hojas de epazote picado \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n30 hojas de maíz para tamales \n', '\n\n\nPara la masa\n\n', '\n\n\n400 gramos de harina de fuerza \n', '\n\n\n125 mililitros de aceite de oliva \n', '\n\n\n125 gramos de azúcar \n', '\n\n\n250 mililitros de agua \n', '\n\n\n1 copa de anís \n', '\n\n\nPara el relleno\n\n', '\n\n\n400 gramos de calabaza \n', '\n\n\n1 puñado de pasas \n', '\n\n\n1 puñado de piñones \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n100 gramos de azúcar (½ taza)\n\n', '\n\n\n2 cucharadas soperas de canela \n', '\n\n\n300 gramos de carne de cerdo (lomo o pierna) \n', '\n\n\n600 gramos de carne de res \n', '\n\n\n1 pechuga de pollo\n\n', '\n\n\n100 gramos de tocino \n', '\n\n\n150 gramos de aceituna verde \n', '\n\n\n25 hojas de bijao\n\n', '\n\n\n2 cebollas blanca mediana\n\n', '\n\n\n½ poro\n\n', '\n\n\n3 ramas de cebollín \n', '\n\n\n4 dientes de ajo\n\n', '\n\n\n20 gramos de alcaparras \n', '\n\n\n2 pimientos rojos\n\n', '\n\n\n30 gramos de pasas \n', '\n\n\n1 taza de vino tinto \n', '\n\n\n1 cucharada sopera de harina de maíz \n', '\nMasa\n', '\n\n\n900 gramos de harina de maíz (7½ tazas)\n\n', '\n\n\n1 taza de agua (240 mililitros)\n\n', '\n\n\n500 gramos de calabaza \n', '\n\n\n80 gramos de queso rallado \n', '\n\n\n1 cebolla\n\n', '\n\n\n1 huevo\n\n', '\n\n\n250 gramos de pan rallado \n', '\n\n\n1 vaso de aceite de oliva \n', '\n\n\n250 gramos de lomo de res \n', '\n\n\n1 cebolla morada mediana\n\n', '\n\n\n1 aji amarillo fresco\n\n', '\n\n\n1 tomate mediano\n\n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n1 cucharada postre de ajo molido \n', '\n\n\n2 chorros de sillao claro \n', '\n\n\n1 pizca de sal \n', '\n\n\n1 huevo\n\n', '\n\n\n1 paquete de pasta de wantán \n', '\n\n\n½ litro de aceite vegetal \n', '\n\n\n1 rama de perejil \n', '\n\n\n200 gramos de queso edam \n', '\n\n\nPara la masa:\n\n', '\n\n\n2 tazas de harina (280 gramos)\n\n', '\n\n\n2½ tazas de agua (600 mililitros)\n\n', '\n\n\n1 cucharada postre de aceite \n', '\n\n\nPara el relleno:\n\n', '\n\n\n10 hojas de albahaca \n', '\n\n\n1 zuchini\n\n', '\n\n\n1 ajo\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 morrón\n\n', '\n\n\n2 huevos\n\n', '\n\n\n2 tomates\n\n', '\n\n\n600 gramos de harina para tamales (harina de maíz nixtamalizada) \n', '\n\n\n2½ tazas de fondo de verduras o agua \n', '\n\n\n200 gramos de manteca vegetal \n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\n1 pizca de sal \n', '\n\n\n3 chiles poblanos\n\n', '\n\n\n2 jitomates\n\n', '\n\n\n1 trozo de cebolla \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 rebanada de cilantro \n', '\n\n\n2 chiles serrano en rajas (opcional)\n\n', '\n\n\nsal y pimienta al gusto\n\n', '\n\n\n300 gramos de queso oaxaca o manchego en tiras o cubos \n', '\n\n\n1 cucharada sopera de aceite \n', '\n\n\n25 hojas de para tamales \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n20 gramos de mantequilla sin sal \n', '\n\n\n130 gramos de queso paria o queso fresco bajo en sal \n', '\n\n\n1 huevo mediano\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1 pizca de pimienta \n', '\n\n\n2 ramas de cebolla china o cebollín \n', '\n\n\n20 gramos de azúcar moreno \n', '\n\n\n10 gramos de polvo de hornear \n', '\n\n\n130 mililitros de agua \n', '\n\n\n5 gramos de anís \n', '\n\n\n5 gramos de levadura seca \n', '\n\n\n15 mililitros de aceite vegetal \n', '\n\n\n1 pizca de sal \n', '\n\n\n250 gramos de harina sin preparar \n', '\n\n\n300 gramos de foie \n', '\n\n\n1 manzanas\n\n', '\n\n\n2 cebollas\n\n', '\n\n\n2 cucharadas soperas de agua \n', '\n\n\n1 cucharada sopera de azúcar(opcional) \n', '\n\n\n2 cucharadas soperas de vinagre balsámico \n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal \n', '\n\n\n500 gramos de papa \n', '\n\n\n1 pizca de sal \n', '\n\n\nagua para cocinar las papas\n\n', '\n\n\n1 cucharadita de mantequilla sin sal \n', '\n\n\n1 cucharada sopera de queso parmesano o queso panela rallado \n', '\n\n\n1 puñado de perejil seco \n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 pizca de pimienta molida \n', '\n\n\n2 huevos\n\n', '\n\n\n2 cucharadas soperas de leche \n', '\n\n\n4 cucharadas soperas de harina de trigo o fécula de maíz \n', '\n\n\n1½ tazas de pan molido o panko \n', '\n\n\n100 granos de queso en cubos \n', '\n\n\n500 mililitros de aceite \n', '\n\n\n2 papas medianas\n\n', '\n\n\n1 huevo\n\n', '\n\n\n½ taza de pan rallado \n', '\n\n\n½ taza de polenta \n', '\n\n\n30 gramos de queso fresco \n', '\n\n\n2 kilogramos de maíz fresco desgranado (choclo) \n', '\n\n\n4 tazas de hojas de culantro \n', '\n\n\n400 gramos de carne de cerdo \n', '\n\n\n1 taza de aceite vegetal \n', '\n\n\n300 gramos de ají amarillo \n', '\n\n\n20 hojas de panca de maíz \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\nPabilo (para amarrar)\n\n', '\n\n\n6 arepas\n\n', '\n\n\n2 muslos de pollo\n\n', '\n\n\n1 aguacate\n\n', '\n\n\n3 cucharadas soperas de mayonesa \n', '\n\n\n1 limón\n\n', '\n\n\n1 cucharadita de orégano \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n½ vaso de vino blanco \n', '\n\n\n6 arepas\n\n', '\n\n\n300 gramos de carne de cerdo o vaca (paleta, falda, tapa de asado) \n', '\n\n\n1 zanahoria\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n¼ pimiento morrón ají verde\n\n', '\n\n\n1 copa de vino \n', '\n\n\n1 diente de ajo \n', '\n\n\n1 hoja de laurel \n', '\n\n\n1 cucharadita de chimichurri o ají molido \n', '\n\n\n1 cucharadita de romero \n', '\n\n\n30 gramos de queso amarillo \n', '\n\n\n1 huevo\n\n', '\n\n\n2 tomates chicos\n\n', '\n\n\n1 cebolla chica\n\n', '\n\n\n¼ pimiento morrón ají rojo\n\n', '\n\n\n½ diente de ajo \n', '\n\n\n2 arepas\n\n', '\n\n\n200 gramos de harina de maíz fina precocida \n', '\n\n\n100 centímetros cúbicos de agua \n', '\n\n\n4 arepas\n\n', '\n\n\n4 filetes de carré\n\n', '\n\n\n1 tomate grande\n\n', '\n\n\n1 cucharada sopera de perejil u orégano seco \n', '\n\n\n500 gramos de choclo o maiz desgranado \n', '\n\n\n1 taza de leche fresca \n', '\n\n\n100 gramos de azucar blanca \n', '\n\n\n1 cucharada postre de anís \n', '\n\n\n50 gramos de mantequilla sin sal \n', '\n\n\n1 chorro de esencia de vainilla \n', '\n\n\n1 puñado de pasas \n', '\n\n\n500 gramos de panca de maiz fresca \n', '\n\n\n300 gramos de harina de maíz (2½ tazas)\n\n', '\n\n\n1 pizca de sal \n', '\n\n\n1½ tazas de agua tibia \n', '\n\n\n1 taza de nopales cocidos picados \n', '\n\n\n1 taza de frijoles refritos \n', '\n\n\n300 gramos de pechuga de pollo cortada en cubos \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n½ cebolla picada\n\n', '\n\n\n1 jitomate picado\n\n', '\n\n\n1 chile serrano picado\n\n', '\n\n\n1 chorro de aceite vegetal \n', '\n\n\n1 puñado de queso rallado al gusto \n', '\n\n\n1 coliflor cocida\n\n', '\n\n\n2 cucharadas soperas de achiote \n', '\n\n\n½ taza de jugo de naranja \n', '\n\n\n2 cucharadas soperas de vinagre \n', '\n\n\n1 chile guajillo limpio\n\n', '\n\n\n1 jitomate\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n1 clavo de olor\n\n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\n\n\n1 trozo de cebolla morada picada \n', '\n\n\n1 cucharadita de aceite \n', '\n\n\nTortillas de maíz\n\n', '\n\n\nCilantro picado\n\n', '\n\n\nTrocitos de piña asada\n\n', '\n\n\nSalsa al gusto\n\n', '\n\n\n400 gramos de setas \n', '\n\n\n1 trozo de cebolla \n', '\n\n\n3 jitomates\n\n', '\n\n\n1 diente de ajo pelado \n', '\n\n\nChile chipotle adobado al gusto\n\n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1 chorro de aceite \n', '\n\n\n½ cebolla blanca fileteada\n\n', '\n\n\n1 pizca de pimienta al gusto \n', '\n\n\n1 pizca de comino en polvo \n', '\n\n\n1½ kilogramos de carne de res para barbacoa \n', '\n\n\n1 pizca de sal al gusto \n', '\n\n\n1½ litros de agua \n', '\n\n\n5 dientes de ajo pelados \n', '\n\n\n5 hojas de laurel \n', '\n\n\n10 pimientas negras enteras\n\n', '\n\n\n1 pizca de orégano seco \n', '\n\n\n1 pizca de tomillo seco \n', '\n\n\n1 pizca de mejorana \n', '\n\n\n1 trozo de cebolla blanca \n', '\n\n\n2 cucharadas soperas de chile quebrado seco (ocpional) \n', '\nPara servir:\n', '\n\n\nCebolla\n\n', '\n\n\nCilantro fresco\n\n', '\n\n\nTortillas de maíz\n\n', '\n\n\nSalsa picante\n\n', '\n\n\nLimón\n\n', '\n\n\n500 gramos de harina de maíz nixtamalizado \n', '\n\n\n100 gramos de harina de trigo o arroz \n', '\n\n\nsal al gusto\n\n', '\n\n\n1 cucharadita de polvo para hornear \n', '\n\n\naceite vegetal\n\n', '\n\n\n400 gramos de pollo desmenuzado \n', '\n\n\n1 cebolla blanca en julianas\n\n', '\n\n\n200 gramos de puré de tomate \n', '\n\n\nsalsa verde para acompañar\n\n', '\n\n\ncrema para acompañar\n\n', '\nPara la salsa tzatziki:\n', '\n\n\n300 gramos de yogur griego \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 diente de ajo en pasta o picado finamente \n', '\n\n\n1 pepino\n\n', '\n\n\n1 chorro de aceite de oliva \n', '\n\n\n1 pizca de sal y pimienta \n', '\n\n\n1 cucharadita de eneldo \n', '\nPara la carne:\n', '\n\n\n500 gramos de pechuga de pollo (también sirve cerdo o cordero) \n', '\n\n\n1 cucharadita de mostaza \n', '\n\n\n1 cucharadita de orégano seco \n', '\n\n\nJugo de medio limón\n\n', '\n\n\n1 pizca de ajo en polvo \n', '\n\n\n1 chorro de aceite \n', '\n\n\n1 pizca de sal y pimienta al gusto \n', '\nPara montar el gyros griego:\n', '\n\n\n5 panes de pita\n\n', '\n\n\n1 tomate en rodajas\n\n', '\n\n\n1 cebolla morada en juliana al gusto\n\n', '\n\n\nHojas de lechuga al gusto\n\n', '\n\n\n1 kilogramo de masa de maíz \n', '\n\n\n2 papas medianas cocidas en puré\n\n', '\n\n\nsal al gusto\n\n', '\n\n\n1 litro de aceite vegetal \n', '\n\n\n400 gramos de carne molida \n', '\n\n\n½ cebolla picada finamente\n\n', '\n\n\n1 docena de ajo picado finamente \n', '\n\n\n80 granos de puré de tomate \n', '\n\n\npimienta al gusto\n\n', '\nPara acompañar\n', '\n\n\ncol blanca (repollo)\n\n', '\n\n\nqueso blanco\n\n', '\n\n\nsalsa picante al gusto\n\n', '\n\n\n1 cebolla\n\n', '\n\n\n1 diente de ajo \n', '\n\n\n3 cucharadas soperas de aceite de oliva \n', '\n\n\n1 pellizco de hebras de azafrán \n', '\n\n\n1 cucharada postre de harina común \n', '\n\n\n1 vaso de vino de Jerez seco \n', '\n\n\n1 kilogramo de almejas \n', '\n\n\n1 rama de perejil \n']</t>
-        </is>
-      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>['\n1\nPara empezar con la receta de champiñones rellenos vegetarianos, primero debes limpiar las verduras y cortar en trozos pequeños la cebolla, el pimiento rojo y el pimiento verde. Seguido, en una sartén vierte un buen chorro de aceite y añade las verduras, deja que se pochen.\n\n\n\n\n\n', '\n2\nLimpia los champiñones con un poco de agua y sécalos enseguida con un papel de cocina. También puedes limpiar con un trapo húmedo y quitarles la tierra. Debes tener cuidado de que no adquieran mucha agua. Seguido, retira el tronco o los tallos de los champiñones y pica en trozos pequeños.\n\n\n\n\n\n', '\n3\nCuando las verduras estén casi pochadas, añade los tronquitos de los champiñones y deja que se cocine todo junto hasta que quede bien pochado. Añade un poco de sal y pimienta. Y, si te gusta, también puedes poner un poquito de orégano o cualquier otra hierva o especia.\n\n\n\n\n\n', '\n4\nColoca los champiñones limpios en una fuente o bandeja para horno y rellena con el sofrito de verduras que has preparado, deben quedar bien rellenos. Enciende el horno para que se caliente a 180 ºC con calor arriba y abajo. ¿Qué te están pareciendo estos champiñones rellenos al horno vegetarianos?\n\n\n\n\n\n', '\n5\nSi lo prefieres, también puedes hacer champiñones rellenos vegetarianos con queso o sin, al gusto. Si te gusta el queso, añade por encima, también puedes incorporar pan rallado, luego, rocía con un poco de aceite de oliva.\n\n\n\n\n\n', '\n6\nColoca la fuente en la parte central del horno a 200 ºC y deja que se cocinen hasta que estén dorados, unos 25 minutos aproximadamente. Cuando estén gratinados, retíralos del horno y sirve enseguida. ¿Qué te ha parecido esta receta de champiñones rellenos de verduras? Déjanos en los comentarios tu opinión.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Champiñones rellenos vegetarianos, te sugerimos que entres en nuestra categoría de Recetas de Setas.\n', '\nChampiñones rellenos veganos\nSi quieres preparar una receta de champiñones veganos, debes cambiar el queso rallado por pan rallado o algún queso vegano. También puedes preparar una bechamel vegana y cubrir los champiñones con ella.Y, si quieres conocer recetas de quesos veganos para añadir en tu elaboración, sigue leyendo:Queso vegano de avenaQueso vegano de anacardosQueso vegano de garbanzosQueso vegano de cacahueteQueso vegano de papa y zanahoria\n', '\nSube la foto de tu Receta de Champiñones rellenos vegetarianos\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta sencilla receta, enjuaga las aceitunas para quitarles la salmuera. A continuación, prepara el resto de los ingredientes en recipientes sepaados: la harina por un lado, el pan rallado por otro y el huevo por otro. También precalienta el horno a temperatura máxima (200 ºC). Luego, rellena las aceitunas con queso, ayudándote con un cuchillo o palillo.\n\n\n\n\n\n', '\n2\nReboza las aceitunas con harina y, luego, pásalas por huevo, pan rallado, huevo y pan rallado nuevamente. Es importante cumplir con el paso de la harina, ya que esta absorbe la humedad de las aceitunas y permite que el huevo y el pan rallado se peguen. En caso de hacer esta preparación para una persona con celiaquía o intolerancia al gluten, considera utilizar una harina sin TACC, así como el resto de ingredientes con el logo pertinente.\n\n\n\n\n\n', '\n3\nDispón las aceitunas rebozadas sobre una bandeja para horno cubierta con la cucharadita de aceite, que puedes distribuir con una servilleta o tu propia mano. Cocínalas en el horno, manteniendo la misma temperatura, durante unos 7-8 minutos. \n\n\n\n\n\n', '\n4\nAhora sí, sirve las aceitunas rebozadas y rellenas con queso bien calientes y disfruta de los hilos de queso en cada mordisco. Como ves, esta receta es ideal para el aperitivo, por lo que te animamos a preparar más platos sencillos para servir un menú completo, como por ejemplo croquetas de calabaza y queso o patatas arrieras. ¡A disfrutar!\n\n\n\n\n\n', '\nSi te ha gustado la receta de Aceitunas rebozadas con queso, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nOtros rellenos para hacer aceitunas rebozadas al horno\nEn lugar de hacer aceitunas rellenas de queso, puedes emplear los siguientes ingredientes:pimiento morróncarne picadaqueso crema con albahacapasta de tomates secos Si te resulta complicado rellenarlas con la mano y un cuchillo o palillo, puedes disponer el relleno en una manga con un corte bien pequeño en la punta para introducirla en el agujero de la aceituna y proceder a rellenarla. En cuanto al rebozado, puedes reemplazar el pan rallado por panko, pero ten en cuenta que tiene más cantidad de grasa. Igualmente, esta preparación reduce varias calorías al estar hecha al horno, respecto a la versión frita.¿Qué te ha parecido esta receta de aceitunas rellenas? Cuéntanos con quién o con qué la compartirías, ¡recomendamos una cerveza bien fría o una copa de vino!\n', '\nSube la foto de tu Receta de Aceitunas rebozadas con queso\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de las arepas venezolanas veganas primero debes mezclar en un bol la harina de maíz blanco precocido, con la sal y el agua (es preferible que las hayas calentado previamente en el microondas o en un cacito). Para que la masa vaya adquiriendo consistencia es recomendable añadir el agua poco a poco para que todos los ingredientes se vayan integrando lo mejor posible.\n\n\n\n\n\n', '\n2\n¡Ha llegado el momento de amasar! Mezcla y amasa para que la harina absorba por completo todo el agua y obtengas una masa lo más compacta posible.\n\n\n\n\n\n', '\n3\nPosteriormente, divide la masa en distintas porciones (en este caso hemos optado por dividir en diez) y elabora pequeñas bolitas para después aplastar con cuidado para lograr la forma redondeada. Es recomendable que cada arepa tenga aproximadamente un centímetro y medio de grosor para poder rellenarlas más tarde.\n\n\n\n\n\n', '\n4\nUna vez hecho el anterior paso, prepara la sartén o la plancha antiadherente. El secreto en este paso está en dejar que las arepas se hagan a fuego lento o a una temperatura media para que se cuezan lo mejor posible por dentro y la masa quede esponjosa. Una vez que se empiecen a dorar por un lado, debes dar la vuelta para que se haga por el otro. Mientras tanto pon el horno a precalentar.\n\n\n\n\n\n', '\n5\nCuando las arepas ya estén listas y mientras preparas el relleno, introduce en el horno a una temperatura también baja para que mantenga el calor y el exterior quede crujiente. Corta las arepas por la mitad sin llegar a separar la tapa de la base para incorporar el relleno. A continuación puedes elegir entre dos propuestas.\n\n\n\n\n\n', '\n6\nPor un lado, pela las cebollas y córtalas en juliana, es decir, en tiras. Posteriormente, incorpora un poco de aceite de oliva en la sartén (preferiblemente antiadherente) y cocina a fuego lento junto a una pizca de sal. Cuando la cebolla pierda gran parte de su volumen y esté prácticamente transparente, añade un par de cucharaditas de azúcar moreno y deja que se siga cocinando lentamente hasta que adquiera el color característico de la cebolla caramelizada.\n', '\n7\nMientras tanto, pela la manzana en dados o tiras y reserva en un bol, en el que tendrás que añadir las nueces también cortadas en trozos pequeños (tres puñados es suficiente). En este mismo recipiente añade el queso feta cortado al gusto, los canónigos y la rúcula (en el caso de que quieras un toque más picante puedes añadir un poco más de rúcula).\n\n\n\n\n\n', '\n8\nPosteriormente, incorpora a la mezcla la cebolla preparada previamente. Para poner el broche final a este relleno mézclalo todo y adereza la mezcla con aceite, sal y vinagre balsámico de Módena. Una vez esté todo listo introdúcelo en las arepas veganas y disfruta. Cuéntanos en los comentarios qué te ha parecido esta receta.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Arepas veganas, te sugerimos que entres en nuestra categoría de Recetas de Arepas. También puedes visitar una selección de las mejores recetas venezolanas.\n', '\nOtros rellenos para las arepas veganas\nNo hay un relleno específico para las arepas, es por eso que en RecetasGratis te animamos a investigar diferentes sabores para lograr tener el relleno perfecto y que más se ajuste a tus necesidades. Un consejo muy importante a la hora de hacer la masa es lograr que esta sea homogénea y evitar que tenga grumos. Si definitivamente quieres sorprender a tus comensales, otra recomendación es añadir a la masa algunos ingredientes, como por ejemplo: semillas de chía, avena o verduras para aumentar el valor nutritivo de la receta, e incluso una cucharada más de azúcar en el caso de utilizar la arepa como postre.Si quieres conocer otras versiones similares, no te pierdas estas recetas saludables:Arepas vegetarianas Arepas de semillas de chía\n', '\nSube la foto de tu Receta de Arepas veganas\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta del pan de ajo keto, primero prepara las hierbas aromáticas. Lava tanto el cebollino como el perejil, sécalo y trocea con un cuchillo afilado. Pela también el diente de ajo y lamínalo. Reserva todos los ingredientes para más adelante.\n\n\n\n\n\n', '\n2\nRalla la bola de mozzarella (también puedes utilizar una mozzarella ya rallada) y colócala en un bol apto para el microondas. Incorpora la almendra molida, el queso crema, el ajo en polvo, la pizca de levadura química y la pizca de sal. Remueve bien, lleva al microondas y calienta 1 minuto a máxima potencia. Retira del microondas y remueve.\n\n\n\n\n\n', '\n3\nBate el huevo como si fuera para una tortilla y añade a la mezcla de pan de ajo keto rápidamente. Remueve para integrar bien.\n\n\n\n\n\n', '\n4\nPrecalienta el horno a 190 ºC y forra una bandeja con papel de horno, pon en él la masa de pan con ajo keto. Con una espátula proporciona forma rectangular, aproximadamente 18x12 cm y un dedo de grosor.\n\n\n\n\n\n', '\n5\nPon las hierbas y el ajo picado que tenías reservado en un bol, incorpora el parmesano rallado y las dos cucharadas de aceite de oliva. Mezcla bien.\n\n\n\n\n\n', '\n6\nCon ayuda de una cucharita, añade esta mezcla encima del pan de ajo keto cubriendo toda la superficie. Hornea el pan a 190 ºC con calor arriba y abajo durante 15 minutos, hasta que esté doradito. El tiempo es orientativo, dependerá de tu horno.\n\n\n\n\n\n', '\n7\nDeja enfriar unos minutos y corta el pan de ajo casero en cuadraditos.\n\n\n\n\n\n', '\n8\nPuedes servir enseguida el pan o puedes consumirlo más tarde. Una vez frío, puedes tostarlo en la tostadora si te gusta más crujiente. Puedes comer el pan de molde keto solo o con salsa de yogur o de mayonesa. Cuéntanos en los comentarios qué te ha parecido esta receta.Espero que te haya gustado la receta y te invito a que visites mi blog Cakes para ti. \n\n\n\n\n\n', '\nSi te ha gustado la receta de Pan de ajo keto, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nPan de ajo versión keto\nSi no sabes qué es la dieta keto, te explicamos que es un tipo de plan alimenticio que se ha puesto de moda en la actualidad para conseguir perder peso rápidamente, aunque no es apta para todo el mundo. Sin embargo, este tipo de pan se puede consumir igualmente si no realizas la dieta keto, ya que esta receta en concreto es muy saludable.Además de este pan que te ofrecemos, existen otras versiones igual de deliciosas, como por ejemplo:Pan de ajo y quesoPan de ajo al hornoY, si quieres conocer más recetas keto, no te pierdas estas elaboraciones fáciles:Pizza keto de polloArroz de coliflor ketoTortillas de queso keto\n', '\nSube la foto de tu Receta de Pan de ajo keto\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con esta receta de torrejas de coliflor, primero lava con abundante agua las verduras. En el caso de la zanahoria, con ayuda de un pelador, retira la piel y rállala. También, corta la cebolla china en rodajas pequeñas, haz lo mismo con la cebolla blanca. Finalmente, retira las semillas del pimiento y corta en cuadrados pequeños.\n\n\n\n\n\n', '\n2\nCon la ayuda de un cuchillo, corta la coliflor y añádela a una olla mediana con agua hirviendo aproximadamente 8-9 minutos. El olor que desprende la coliflor al ser cocida suele ser desagradable para muchas personas, pero existe un truco para deshacerse de ese particular olor, toma nota: en el momento de cocinar la coliflor, agrega 1 chorro de vinagre blanco.\n\n\n\n\n\n', '\n3\nPasado el tiempo, retira la coliflor y reserva en un recipiente de metal.\n\n\n\n\n\n', '\n4\nSepara la yema de los huevos y con la ayuda de un batidor eléctrico o manual, bate las claras hasta llegar a un punto nieve.\n\n\n\n\n\n', '\n5\nEn un recipiente mediano, añade las verduras picadas y la coliflor. Mezcla con las cuatro yemas de huevo.\n\n\n\n\n\n', '\n6\nCon una cuchara mezcla las claras a punto nieve, es importante mezclar de manera envolvente para evitar la pérdida de aire. ¿Qué te están pareciendo estas torrejas de coliflor sin harina?\n\n\n\n\n\n', '\n7\nColoca una sartén caliente a fuego medio con un chorro de aceite y añade una cuchara de mezcla, cocina hasta que se encuentre dorada la torreja de coliflor.\n\n\n\n\n\n', '\n8\nYa están listas las torrejas de coliflor fritas, sirve con arroz o salsa peruana. Señalamos que también puedes elaborar bolitas de coliflor si no quieres elaborar las torrejas planas. Cuéntanos en los comentarios qué te ha parecido esta receta peruana.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Torrejas de coliflor, te sugerimos que entres en nuestra categoría de Recetas de Otros aperitivos.\n', '\nTorrejas de coliflor al horno\nSi cocinas estos fritos de coliflor al horno, solo debes intercambiar el paso de la fritura en la sartén y colocar las torrejas en una bandeja metálica para introducir en el horno aproximadamente 10 minutos a 170 ºC. Ten en cuenta que debes revisarlas continuamente para que no se quemen. La cocción en el horno harán de esta receta una elaboración mucho más saludable. Además, el consumo de coliflor es beneficioso para la salud, es una importante fuente de fibra que ayuda a la absorción de hierro. Por cada 100 gramos de coliflor se encuentran: 25 calorías, 3g de fibra, 77% de vitamina C, 20% de vitamina K, potasio, manganeso, ácido pantoténico y fósforo.Si quieres conocer más recetas con coliflor, no te pierdas las siguientes elaboraciones:Albóndigas de coliflorNuggets de coliflor veganosCroquetas de coliflor al hornoTortilla de coliflor\n', '\nSube la foto de tu Receta de Torrejas de coliflor\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de tamales de piña con coco, limpia bien las hojas para tamal y remoja en agua caliente para que se suavicen aproximadamente unos 20 o 30 minutos.\n\n\n\n\n\n', '\n2\nPara la masa de los tamales, en un bol mezcla la harina de maíz con el agua y remueve. Después, agrega el azúcar, el polvo para hornear, la canela y la vainilla, integra todo muy bien.\n\n\n\n\n\n', '\n3\nLuego, licua la piña en trozo con unas 2 cucharadas de coco rallado y almíbar o jugo de piña para formar una pasta ligeramente aguada.\n\n\n\n\n\n', '\n4\nCuando tengas la piña licuada, vacía en el bol de la masa y agrega también la mantequilla. Mezcla hasta incorporar por completo, debe quedar una masa muy húmeda, pero también firme.\n\n\n\n\n\n', '\n5\nPor último, agrega el resto del coco rallado y mezcla una vez más para que el coco se integre en la masa.\n\n\n\n\n\n', '\n6\nAhora es momento de armar los tamales. Toma una hoja y agrega una porción de la masa, distribuye de centro hacia arriba, envuelve y cierra bien el tamal, seguido, acomoda en una olla vaporera, luego, lleva a cocinar aproximadamente 1 hora a fuego medio. ¿Qué te están pareciendo estos tamales con mantequilla?\n\n\n\n\n\n', '\n7\nPara saber si los tamales dulces de piña están listos, revisa uno y si la hoja se desprende fácil, ya estarán listos para disfrutar. Sirve acompañado de un rico atole de coco o vainilla. Cuéntanos en los comentarios qué te han parecido estos tamales de dulce con piña y coco.\n\n\n\n\n\n', '\nSi te ha gustado la receta de Tamales de piña con coco, te sugerimos que entres en nuestra categoría de Recetas de Tamales. También puedes visitar una selección de las mejores recetas mexicanas.\n', '\nTamales de piña con coco y otros ingredientes\nPreparar tamales nunca ha sido complicado, la verdad es que es muy sencillo y si sigues nuestra receta, estos tamales de piña con coco te quedarán riquísimos. Además, otros ingredientes que puedes agregar a estos tamales son: nuez, plátano, chocolate, entre otros. Señalamos que los tamales de piña con coco y pasas también están deliciosos, así pues, puedes añadir un puñado de pasas. Además, también puedes probar añadiendo un relleno de queso crema o dulce de leche. ¿Y con qué acompañar los tamales de piña y coco? No olvides que un buen tamal se disfruta más con un rico atole, con un café de olla o con un chocolate caliente. Así que anímate a preparar esta elaboración y prueba también con alguna de nuestras recetas fáciles de atole, seguro habrá alguna que te gusta:Atole de pinoleAtole de maízAtole de fresaAtole con piloncilloAtole de guayabaAtole de amarantoY, si quieres conocer más recetas de tamales, no te pierdas estas elaboraciones:Tamales de NutellaTamales de calabazaTamales de elote dulcesTamales de frijolesTamales de dulceTamales canarios\n', '\nSube la foto de tu Receta de Tamales de piña con coco\n\n\n\nSube la foto de tu plato \n\n\n', '\n1\nPara empezar con la receta de empanadas de hamburguesa, primero debes hacer la cebolla. Para ello, pélala, pícala y saltéala con 1 cucharadita de aceite en una sartén a fuego fuerte. Cuando esté dorada, baja el fuego a medio y agrega 1 cucharada de agua caliente. En cuanto el agua se evapore, agrega una cucharada nuevamente. Repite el proceso tantas veces como quieras sabiendo que, cuantas más veces lo hagas, más dulces y caramelizadas quedarán.\n\n\n\n\n\n', '\n2\nUna vez que la cebolla esté lista, sube el fuego a alto y, cuando la sartén tome temperatura, agrega 25 cc de vino. Reserva para que no sientas más olor ácido del alcohol y apaga el fuego. Retira y reserva.\n\n\n\n\n\n', '\n3\nUtiliza el fondo de cocción de la cebolla para dorar la carne picada. Hazlo en tandas para que no libere mucho jugo y se dore de forma pareja. Señalamos que no es necesario que la cocines completamente, pues también la cocinarás dentro del horno, pero es importante que se dore para que tome sabor.\n\n\n\n\n\n', '\n4\nMezcla la carne con la cebolla salteada previamente y condimentos al gusto: comino, pimentón ahumado y ají molido. Deja que el relleno de tus empanadas de hamburguesa se enfríe. Puedes hacerlo a temperatura ambiente, asegurándote que no pasen más de 2 horas o también puedes hacerlo en heladera, y si puedes dejarlo enfriar de un día para el otro, tendrá mucho más sabor.\n\n\n\n\n\n', '\n5\nUna vez que el relleno esté listo, comienza a armar tus empanadas de hamburguesas. Para ello, humedece con el dedo el borde del disco y unta la mitad con el queso cheddar